<commit_message>
magnify the armature of leg, robot does not squat forever.
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -611,82 +611,82 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>-7.925473025143468e-05</v>
+        <v>1.799050066851663e-05</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>-1.111730743271269e-15</v>
+        <v>9.26442286059391e-17</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>1.706187263092052e-05</v>
+        <v>3.026177118578045e-05</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>-5.823351512373315e-16</v>
+        <v>1.919059021123024e-16</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>-2.130371624514218e-05</v>
+        <v>1.496858551907218e-05</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>2.32998302877666e-06</v>
+        <v>6.105136086874828e-06</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>5.139280742777525e-06</v>
+        <v>1.232255564956728e-07</v>
       </c>
       <c r="K2" s="3" t="n">
-        <v>7.146840492458159e-16</v>
+        <v>0</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>-2.130371624937735e-05</v>
+        <v>1.496858551901924e-05</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>2.329983028088446e-06</v>
+        <v>6.105136086785492e-06</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>5.139280745980369e-06</v>
+        <v>1.232255558537806e-07</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>1.455837878093329e-15</v>
+        <v>0</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>0.001998867736902079</v>
+        <v>0.001998018843353699</v>
       </c>
       <c r="Q2" t="n">
-        <v>-4.235164736271502e-16</v>
+        <v>-1.985233470127266e-16</v>
       </c>
       <c r="R2" t="n">
-        <v>-2.465466882279112e-06</v>
+        <v>5.418022901891489e-07</v>
       </c>
       <c r="S2" t="n">
-        <v>-8.735027268559972e-16</v>
+        <v>5.856438736875436e-16</v>
       </c>
       <c r="T2" t="n">
-        <v>1.760177900508669e-07</v>
+        <v>3.170844034733207e-07</v>
       </c>
       <c r="U2" t="n">
-        <v>-3.705769144237564e-16</v>
+        <v>5.293955920339377e-17</v>
       </c>
       <c r="V2" t="n">
-        <v>-3.833158146670395e-06</v>
+        <v>1.569305089475849e-07</v>
       </c>
       <c r="W2" t="n">
-        <v>-9.841550821201458e-08</v>
+        <v>6.384179521337609e-08</v>
       </c>
       <c r="X2" t="n">
-        <v>2.394370936905559e-07</v>
+        <v>1.356982846576096e-11</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.222415991128764e-08</v>
+        <v>2.958130122442068e-08</v>
       </c>
       <c r="Z2" t="n">
-        <v>-3.833158146564516e-06</v>
+        <v>1.569305087788401e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>-9.841550770908877e-08</v>
+        <v>6.384179600416076e-08</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.394370934523278e-07</v>
+        <v>1.356939833184244e-11</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.222416033480412e-08</v>
+        <v>2.958130116817239e-08</v>
       </c>
     </row>
     <row r="3">
@@ -696,88 +696,88 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>2.8317493839997e-15</v>
+        <v>3.219509513749243e-18</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>2.025166027501004e-15</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.000560110595907754</v>
+        <v>3.055885859484022e-16</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0.001489466485253299</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>-5.107800925295806e-16</v>
+        <v>8.421459735278193e-17</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>4.046082559643129e-07</v>
+        <v>-5.519062642971246e-08</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>-1.240393552479856e-05</v>
+        <v>2.758261440566211e-05</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>-0.0001122260931874908</v>
+        <v>-0.0005647066910612514</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>3.458311443867404e-05</v>
+        <v>9.791951507300594e-08</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>-2.847159915362051e-16</v>
+        <v>1.52680729448644e-26</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>1.240393552372425e-05</v>
+        <v>-2.758261440538667e-05</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>0.0001122260931907737</v>
+        <v>0.0005647066910606479</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>-3.458311442821735e-05</v>
+        <v>-9.791951347700811e-08</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>-7.128348747609055e-15</v>
+        <v>1.526826102396053e-26</v>
       </c>
       <c r="P3" t="n">
-        <v>2.06085158165588e-15</v>
+        <v>-6.12476983237632e-16</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>0.001902162674964758</v>
+        <v>0.001719550529941815</v>
       </c>
       <c r="R3" t="n">
-        <v>-1.641852939518401e-15</v>
+        <v>6.582655066444399e-17</v>
       </c>
       <c r="S3" t="n">
-        <v>9.698362673398309e-07</v>
+        <v>8.73012199837392e-07</v>
       </c>
       <c r="T3" t="n">
-        <v>-5.406645667548855e-15</v>
+        <v>7.855749671043616e-16</v>
       </c>
       <c r="U3" t="n">
-        <v>1.410042934505758e-06</v>
+        <v>5.762065200008456e-08</v>
       </c>
       <c r="V3" t="n">
-        <v>-9.649058406158782e-06</v>
+        <v>3.91980588624998e-07</v>
       </c>
       <c r="W3" t="n">
-        <v>-2.105117575951649e-06</v>
+        <v>-1.742984648754667e-05</v>
       </c>
       <c r="X3" t="n">
-        <v>2.221188971489806e-06</v>
+        <v>4.13393986383874e-09</v>
       </c>
       <c r="Y3" t="n">
-        <v>2.077026085425754e-07</v>
+        <v>-8.479805312652762e-08</v>
       </c>
       <c r="Z3" t="n">
-        <v>9.649058411654869e-06</v>
+        <v>-3.919805869990077e-07</v>
       </c>
       <c r="AA3" t="n">
-        <v>2.105117579284658e-06</v>
+        <v>1.742984648706186e-05</v>
       </c>
       <c r="AB3" t="n">
-        <v>-2.221188975083157e-06</v>
+        <v>-4.133940625313281e-09</v>
       </c>
       <c r="AC3" t="n">
-        <v>-2.077026050447135e-07</v>
+        <v>8.479805395969846e-08</v>
       </c>
     </row>
     <row r="4">
@@ -793,82 +793,82 @@
         <v>0</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.9921172491669794</v>
+        <v>0.9873663694009993</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-1.827618612004756e-05</v>
+        <v>-2.380758090669843e-05</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>1.709299368712891e-06</v>
+        <v>-1.910798602677843e-05</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>0.0001308316371906315</v>
+        <v>0.0003869579379145449</v>
       </c>
       <c r="J4" s="3" t="n">
-        <v>-4.452740259841548e-05</v>
+        <v>-6.905587213168474e-08</v>
       </c>
       <c r="K4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>1.709299368712891e-06</v>
+        <v>-1.910798602677843e-05</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>0.0001308316371906315</v>
+        <v>0.0003869579379145449</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>-4.452740259841548e-05</v>
+        <v>-6.905587213168474e-08</v>
       </c>
       <c r="O4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>1.02281863534337e-05</v>
+        <v>-4.757659544107895e-06</v>
       </c>
       <c r="Q4" t="n">
         <v>0</v>
       </c>
       <c r="R4" s="4" t="n">
-        <v>0.001771560134700145</v>
+        <v>0.001615194096526995</v>
       </c>
       <c r="S4" t="n">
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>-2.055314252125129e-06</v>
+        <v>4.491546023999149e-08</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
       </c>
       <c r="V4" t="n">
-        <v>1.157043905131161e-05</v>
+        <v>-2.011446564864627e-07</v>
       </c>
       <c r="W4" t="n">
-        <v>2.645689223257364e-06</v>
+        <v>1.198112442590826e-05</v>
       </c>
       <c r="X4" t="n">
-        <v>-2.87379842145441e-06</v>
+        <v>-2.844946500601964e-09</v>
       </c>
       <c r="Y4" t="n">
-        <v>-1.346422973114159e-07</v>
+        <v>7.085998454670062e-08</v>
       </c>
       <c r="Z4" t="n">
-        <v>1.157043905131161e-05</v>
+        <v>-2.011446564864627e-07</v>
       </c>
       <c r="AA4" t="n">
-        <v>2.645689223257364e-06</v>
+        <v>1.198112442590826e-05</v>
       </c>
       <c r="AB4" t="n">
-        <v>-2.87379842145441e-06</v>
+        <v>-2.844946500601964e-09</v>
       </c>
       <c r="AC4" t="n">
-        <v>-1.346422973114159e-07</v>
+        <v>7.085998454670062e-08</v>
       </c>
     </row>
     <row r="5">
@@ -878,88 +878,88 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>2.597377399509766e-13</v>
+        <v>1.673052754524455e-14</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>1.305856527945283e-15</v>
+        <v>2.301517696593952e-16</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-1.072183975697882e-13</v>
+        <v>-1.860739918528885e-14</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.9958900634972051</v>
+        <v>0.9892438482012174</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>-1.246626409155828e-13</v>
+        <v>-1.267855515205999e-14</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>-2.335333822067455e-05</v>
+        <v>3.944223926405342e-07</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>0.0001442685504712879</v>
-      </c>
-      <c r="I5" s="3" t="n">
-        <v>0.0008786814717452686</v>
+        <v>-0.0001991766102041677</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>0.004078041405273314</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>-0.0002573385807856253</v>
+        <v>-6.920746785633278e-07</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>1.349663770004712e-13</v>
+        <v>6.520669004974354e-18</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>-0.0001442685505350851</v>
-      </c>
-      <c r="M5" s="3" t="n">
-        <v>-0.0008786814717746054</v>
+        <v>0.0001991766102019097</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>-0.004078041405225986</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>0.0002573385807796418</v>
+        <v>6.920745941750811e-07</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>1.776043070569432e-13</v>
+        <v>6.520669004974354e-18</v>
       </c>
       <c r="P5" t="n">
-        <v>-1.852562248356706e-13</v>
-      </c>
-      <c r="Q5" s="4" t="n">
-        <v>-0.001807660335720352</v>
+        <v>2.259898497556936e-14</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0.0005333499460042509</v>
       </c>
       <c r="R5" t="n">
-        <v>-8.908787386006739e-15</v>
+        <v>-1.871774857139237e-15</v>
       </c>
       <c r="S5" s="4" t="n">
-        <v>0.001586887320813219</v>
+        <v>0.001585491060066447</v>
       </c>
       <c r="T5" t="n">
-        <v>1.801568950510391e-13</v>
+        <v>-3.044364980132614e-14</v>
       </c>
       <c r="U5" t="n">
-        <v>-8.734016647898417e-06</v>
+        <v>-9.112615318588796e-07</v>
       </c>
       <c r="V5" t="n">
-        <v>7.540040140565317e-05</v>
+        <v>-7.921354765130119e-06</v>
       </c>
       <c r="W5" t="n">
-        <v>1.602708571404251e-05</v>
+        <v>0.0001232485069633201</v>
       </c>
       <c r="X5" t="n">
-        <v>-1.644942824140504e-05</v>
+        <v>-2.921764308563011e-08</v>
       </c>
       <c r="Y5" t="n">
-        <v>-1.95195552522763e-06</v>
+        <v>-3.485488296203241e-07</v>
       </c>
       <c r="Z5" t="n">
-        <v>-7.540040192894597e-05</v>
+        <v>7.92135468909651e-06</v>
       </c>
       <c r="AA5" t="n">
-        <v>-1.602708550940064e-05</v>
+        <v>-0.0001232485069610224</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.644942848162176e-05</v>
+        <v>2.921765670585524e-08</v>
       </c>
       <c r="AC5" t="n">
-        <v>1.951955422967899e-06</v>
+        <v>3.485488156246421e-07</v>
       </c>
     </row>
     <row r="6">
@@ -974,83 +974,83 @@
       <c r="C6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>-0.01475239317649838</v>
+      <c r="D6" s="3" t="n">
+        <v>8.241215373854961e-05</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>1.640807287493841e-13</v>
+        <v>3.71210784615423e-15</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1.000223315330629</v>
+        <v>1.00021910609572</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>2.123283852059545e-13</v>
-      </c>
-      <c r="H6" s="2" t="n">
-        <v>0.004121418103926274</v>
-      </c>
-      <c r="I6" s="2" t="n">
-        <v>0.00221428400812755</v>
+        <v>7.265081096321951e-15</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>0.000108788260404134</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>4.660869657367959e-05</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>-1.649226611535366e-06</v>
+        <v>1.488720431516092e-06</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="L6" s="2" t="n">
-        <v>0.004121418104393835</v>
-      </c>
-      <c r="M6" s="2" t="n">
-        <v>0.002214284007959838</v>
+      <c r="L6" s="3" t="n">
+        <v>0.0001087882604022811</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>4.660869656256229e-05</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>-1.649226858868986e-06</v>
+        <v>1.488720415369527e-06</v>
       </c>
       <c r="O6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P6" s="4" t="n">
-        <v>0.002137689424728818</v>
+        <v>0.002541966837551584</v>
       </c>
       <c r="Q6" t="n">
-        <v>-2.21834497932223e-13</v>
+        <v>-7.23969442799065e-15</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.0003788487148501717</v>
+        <v>3.861834686948845e-06</v>
       </c>
       <c r="S6" t="n">
-        <v>1.231008743579555e-14</v>
+        <v>2.198477445315336e-14</v>
       </c>
       <c r="T6" s="4" t="n">
-        <v>0.001658340557199947</v>
+        <v>0.001594455129139282</v>
       </c>
       <c r="U6" t="n">
-        <v>1.008562622327013e-13</v>
+        <v>1.888425185228826e-15</v>
       </c>
       <c r="V6" t="n">
-        <v>0.0002854624842801927</v>
+        <v>-0.0002005771877196362</v>
       </c>
       <c r="W6" t="n">
-        <v>-1.139653067304491e-06</v>
+        <v>-0.0001033384706157853</v>
       </c>
       <c r="X6" t="n">
-        <v>5.515909795728343e-06</v>
+        <v>2.526593204669833e-08</v>
       </c>
       <c r="Y6" t="n">
-        <v>-2.882089615164025e-05</v>
+        <v>-3.786088037811842e-05</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.0002854624843191562</v>
+        <v>-0.0002005771877023249</v>
       </c>
       <c r="AA6" t="n">
-        <v>-1.139652708162521e-06</v>
+        <v>-0.000103338470594186</v>
       </c>
       <c r="AB6" t="n">
-        <v>5.515909844856255e-06</v>
+        <v>2.526590830330602e-08</v>
       </c>
       <c r="AC6" t="n">
-        <v>-2.882089601950311e-05</v>
+        <v>-3.786088037232153e-05</v>
       </c>
     </row>
     <row r="7">
@@ -1066,82 +1066,82 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>5.198473657290252e-14</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>-0.001508495651119861</v>
+        <v>9.31667374088876e-15</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>-0.0001348875954676646</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>-1.602996375963263e-14</v>
+        <v>-2.124715093493255e-14</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.999999999726686</v>
-      </c>
-      <c r="H7" s="2" t="n">
-        <v>0.004085758489429281</v>
-      </c>
-      <c r="I7" s="2" t="n">
-        <v>0.002127682397340212</v>
+        <v>0.9999999999999228</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <v>-1.708122517529066e-06</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>5.275683340555578e-05</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>-9.920149726341674e-05</v>
+        <v>1.096503081774268e-06</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="L7" s="2" t="n">
-        <v>-0.004085758489390006</v>
-      </c>
-      <c r="M7" s="2" t="n">
-        <v>-0.002127682397520294</v>
+      <c r="L7" s="3" t="n">
+        <v>1.708122518862741e-06</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>-5.275683339151776e-05</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>9.920149721406272e-05</v>
+        <v>-1.096503096111955e-06</v>
       </c>
       <c r="O7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>-1.96034486686006e-14</v>
+        <v>-3.305523206341751e-15</v>
       </c>
       <c r="Q7" t="n">
-        <v>-0.0001132524291075111</v>
+        <v>-7.989363723988109e-06</v>
       </c>
       <c r="R7" t="n">
-        <v>1.421493181358672e-14</v>
+        <v>7.661134816082269e-15</v>
       </c>
       <c r="S7" t="n">
-        <v>-5.796778672365525e-05</v>
+        <v>-5.18812141603735e-06</v>
       </c>
       <c r="T7" t="n">
-        <v>-2.320742029727915e-14</v>
+        <v>-1.487829301971499e-14</v>
       </c>
       <c r="U7" s="4" t="n">
-        <v>0.001797287268822461</v>
+        <v>0.001614896055877996</v>
       </c>
       <c r="V7" t="n">
-        <v>0.0003239614470837472</v>
+        <v>-0.0003739430180996966</v>
       </c>
       <c r="W7" t="n">
-        <v>1.696469256856013e-06</v>
+        <v>-0.0001909196171588882</v>
       </c>
       <c r="X7" t="n">
-        <v>1.633667417912313e-08</v>
+        <v>4.630011212946275e-08</v>
       </c>
       <c r="Y7" t="n">
-        <v>-2.77373732474923e-05</v>
+        <v>-7.057116844418313e-05</v>
       </c>
       <c r="Z7" t="n">
-        <v>-0.0003239614471563588</v>
+        <v>0.00037394301810578</v>
       </c>
       <c r="AA7" t="n">
-        <v>-1.696469095088494e-06</v>
+        <v>0.0001909196171594517</v>
       </c>
       <c r="AB7" t="n">
-        <v>-1.633668364003253e-08</v>
+        <v>-4.630009844725853e-08</v>
       </c>
       <c r="AC7" t="n">
-        <v>2.7737373254507e-05</v>
+        <v>7.057116846065799e-05</v>
       </c>
     </row>
     <row r="8">
@@ -1151,88 +1151,88 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>-1.761828530288945e-13</v>
+        <v>2.358757215483243e-19</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>-0.03094735254362556</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>-0.004839288107276452</v>
+        <v>-3.231174267785264e-21</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>3.263908748192953e-07</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>3.136744661880054e-08</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>-3.424318234567306e-05</v>
+        <v>1.662620320939083e-09</v>
       </c>
       <c r="G8" s="3" t="n">
-        <v>-8.809142651444724e-14</v>
+        <v>6.086239850800324e-17</v>
       </c>
       <c r="H8" s="2" t="n">
-        <v>0.9928108114049822</v>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>0.001639040830257743</v>
+        <v>0.9999992878965601</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>-3.47472851415827e-07</v>
       </c>
       <c r="J8" s="3" t="n">
-        <v>0.0006652387249121336</v>
+        <v>-2.617893891926138e-08</v>
       </c>
       <c r="K8" s="3" t="n">
-        <v>1.965116437629977e-13</v>
-      </c>
-      <c r="L8" s="2" t="n">
-        <v>-0.001687618379677541</v>
-      </c>
-      <c r="M8" s="2" t="n">
-        <v>-0.001314723319463171</v>
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>-9.872059721734802e-09</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>-3.205527506378042e-09</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>0.0001514100076463161</v>
+        <v>-1.092574880428599e-10</v>
       </c>
       <c r="O8" s="3" t="n">
-        <v>1.897353801849633e-13</v>
+        <v>0</v>
       </c>
       <c r="P8" t="n">
-        <v>0.0001039823784666554</v>
-      </c>
-      <c r="Q8" s="4" t="n">
-        <v>0.001018830163633619</v>
+        <v>1.289817072710992e-08</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.133343533989182e-08</v>
       </c>
       <c r="R8" t="n">
-        <v>-0.000894687329390108</v>
+        <v>9.94825355865961e-09</v>
       </c>
       <c r="S8" t="n">
-        <v>2.687727003577913e-05</v>
+        <v>2.806195377350718e-09</v>
       </c>
       <c r="T8" t="n">
-        <v>-1.824532462369214e-05</v>
+        <v>-2.039345674979021e-09</v>
       </c>
       <c r="U8" t="n">
-        <v>-6.459869728844608e-05</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0.0009445695058638102</v>
+        <v>-8.542041465607908e-09</v>
+      </c>
+      <c r="V8" s="4" t="n">
+        <v>0.001999920903326038</v>
       </c>
       <c r="W8" t="n">
-        <v>-3.178956122456113e-05</v>
+        <v>-2.056551441794267e-08</v>
       </c>
       <c r="X8" t="n">
-        <v>3.304680283626937e-05</v>
+        <v>-1.10716648425008e-09</v>
       </c>
       <c r="Y8" t="n">
-        <v>-1.462983207479009e-05</v>
+        <v>-2.176229986960578e-09</v>
       </c>
       <c r="Z8" t="n">
-        <v>-0.0001552743567336218</v>
+        <v>9.492112961880812e-09</v>
       </c>
       <c r="AA8" t="n">
-        <v>-8.380503119264672e-06</v>
+        <v>4.924098344729893e-09</v>
       </c>
       <c r="AB8" t="n">
-        <v>7.483776111023941e-06</v>
+        <v>-1.211633236183117e-12</v>
       </c>
       <c r="AC8" t="n">
-        <v>1.177899933894975e-05</v>
+        <v>1.792011796281027e-09</v>
       </c>
     </row>
     <row r="9">
@@ -1242,88 +1242,88 @@
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>7.589415207398531e-13</v>
+        <v>0</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D9" s="2" t="n">
-        <v>0.08817536740891148</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>0.01127794622873325</v>
+      <c r="D9" s="3" t="n">
+        <v>3.463343045055214e-06</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>8.203946815456024e-07</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>0.0001688777684317674</v>
+        <v>5.214270636563481e-09</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>2.981555974335137e-13</v>
+        <v>2.729696021424991e-16</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>0.0006858820306143969</v>
+        <v>-3.05956075888847e-07</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>0.9897393747841492</v>
-      </c>
-      <c r="J9" s="2" t="n">
-        <v>-0.001190572867723616</v>
+        <v>0.9999968550265748</v>
+      </c>
+      <c r="J9" s="3" t="n">
+        <v>-2.334589114533663e-06</v>
       </c>
       <c r="K9" s="3" t="n">
-        <v>2.710505431213761e-13</v>
+        <v>0</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>-0.0001578095710748698</v>
+        <v>-1.591263566372688e-08</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>0.0008391529214665967</v>
+        <v>2.169820031841313e-07</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>-0.0003343014364409671</v>
+        <v>-9.702909566228984e-11</v>
       </c>
       <c r="O9" s="3" t="n">
-        <v>-1.897353801849633e-13</v>
+        <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>0.0002589122082420452</v>
-      </c>
-      <c r="Q9" s="4" t="n">
-        <v>-0.002004738539128186</v>
-      </c>
-      <c r="R9" s="4" t="n">
-        <v>0.002562001546080762</v>
+        <v>1.671929032373808e-08</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1.455641722021424e-07</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.054961148597646e-07</v>
       </c>
       <c r="S9" t="n">
-        <v>1.298787981459867e-06</v>
+        <v>1.27610161018132e-09</v>
       </c>
       <c r="T9" t="n">
-        <v>-3.654125271682421e-05</v>
+        <v>-2.471656978881057e-09</v>
       </c>
       <c r="U9" t="n">
-        <v>-1.875881305217313e-05</v>
+        <v>-5.607478631865898e-09</v>
       </c>
       <c r="V9" t="n">
-        <v>0.0002969694147167933</v>
+        <v>-2.151787339631174e-08</v>
       </c>
       <c r="W9" s="4" t="n">
-        <v>0.001662809808572994</v>
+        <v>0.001999869072171175</v>
       </c>
       <c r="X9" t="n">
-        <v>-7.70524145518852e-05</v>
+        <v>-9.857633706838063e-08</v>
       </c>
       <c r="Y9" t="n">
-        <v>-7.312697946097388e-06</v>
+        <v>-1.543499344397177e-09</v>
       </c>
       <c r="Z9" t="n">
-        <v>7.612168371768507e-05</v>
+        <v>5.21224342864035e-09</v>
       </c>
       <c r="AA9" t="n">
-        <v>1.920133572540922e-05</v>
+        <v>9.530991669673302e-09</v>
       </c>
       <c r="AB9" t="n">
-        <v>-2.178074138148994e-05</v>
+        <v>-2.293704009799316e-12</v>
       </c>
       <c r="AC9" t="n">
-        <v>4.34707039245405e-07</v>
+        <v>1.045498471860668e-09</v>
       </c>
     </row>
     <row r="10">
@@ -1333,88 +1333,88 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>8.131516293641283e-13</v>
+        <v>2.584939414228211e-20</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="n">
-        <v>-0.08877877789043184</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>-0.01134281214844345</v>
+      <c r="D10" s="3" t="n">
+        <v>-2.682473495223039e-08</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>-1.553283351492538e-09</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>-0.0001699663720313924</v>
+        <v>1.712607203515174e-11</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>1.273937552670468e-12</v>
+        <v>2.257427590445497e-16</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>-0.0007399770685524026</v>
+        <v>-2.616350380813675e-08</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>0.0004759166660479701</v>
+        <v>-2.333208910938967e-06</v>
       </c>
       <c r="J10" s="2" t="n">
-        <v>0.9918185838372071</v>
+        <v>0.9999978124899631</v>
       </c>
       <c r="K10" s="3" t="n">
-        <v>-1.626303258728257e-13</v>
+        <v>0</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0.0001744537499214546</v>
+        <v>-6.251472392529953e-11</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>-0.0008367095679230174</v>
+        <v>2.064041141083864e-10</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>0.000335140722763699</v>
+        <v>-6.757694794999265e-13</v>
       </c>
       <c r="O10" s="3" t="n">
-        <v>-1.626303258728257e-13</v>
+        <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>-0.0002598870748053879</v>
-      </c>
-      <c r="Q10" s="4" t="n">
-        <v>0.002012270912887196</v>
-      </c>
-      <c r="R10" s="4" t="n">
-        <v>-0.002579516506726878</v>
+        <v>3.195981722381248e-10</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-3.371255126063428e-11</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-8.168524956860907e-10</v>
       </c>
       <c r="S10" t="n">
-        <v>-1.959953548199764e-06</v>
+        <v>-5.274827806175084e-11</v>
       </c>
       <c r="T10" t="n">
-        <v>3.666423769948211e-05</v>
+        <v>-5.250546361964465e-11</v>
       </c>
       <c r="U10" t="n">
-        <v>1.902702087140835e-05</v>
+        <v>-1.005286727456039e-10</v>
       </c>
       <c r="V10" t="n">
-        <v>-0.0002940384650172712</v>
+        <v>-1.233377795119541e-09</v>
       </c>
       <c r="W10" t="n">
-        <v>-7.741335328846632e-05</v>
+        <v>-9.860049442631637e-08</v>
       </c>
       <c r="X10" s="4" t="n">
-        <v>0.001690380376255171</v>
+        <v>0.001999908919840294</v>
       </c>
       <c r="Y10" t="n">
-        <v>7.394739036598388e-06</v>
+        <v>-2.314133745002485e-11</v>
       </c>
       <c r="Z10" t="n">
-        <v>-7.49527340150255e-05</v>
+        <v>7.181677086987321e-11</v>
       </c>
       <c r="AA10" t="n">
-        <v>-1.923162952673085e-05</v>
+        <v>4.413814644491343e-11</v>
       </c>
       <c r="AB10" t="n">
-        <v>2.185880944023492e-05</v>
+        <v>-1.076772022633247e-14</v>
       </c>
       <c r="AC10" t="n">
-        <v>-5.013913817551036e-07</v>
+        <v>1.362028328426417e-11</v>
       </c>
     </row>
     <row r="11">
@@ -1424,88 +1424,88 @@
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>-1.10114283143059e-13</v>
+        <v>3.722312756488625e-18</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <v>-0.008335147706639042</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>-0.001344087940978046</v>
+      <c r="D11" s="3" t="n">
+        <v>-2.361791920797229e-06</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>8.154841151832739e-06</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>-0.0002184211800142222</v>
+        <v>-3.85872407470422e-06</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-3.574479037413147e-13</v>
-      </c>
-      <c r="H11" s="2" t="n">
-        <v>0.002061425300063633</v>
-      </c>
-      <c r="I11" s="2" t="n">
-        <v>0.001953138813088303</v>
+        <v>-2.067951531382569e-18</v>
+      </c>
+      <c r="H11" s="3" t="n">
+        <v>-1.752680562429738e-06</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>-3.857794473732625e-06</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>0.0001207042668669844</v>
+        <v>-6.418436552602937e-09</v>
       </c>
       <c r="K11" s="2" t="n">
-        <v>1.00000000000009</v>
-      </c>
-      <c r="L11" s="2" t="n">
-        <v>-0.001603803177797767</v>
+        <v>1</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>-2.063931440004631e-06</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>-0.0009093289685468351</v>
+        <v>2.308790164670931e-06</v>
       </c>
       <c r="N11" s="3" t="n">
-        <v>2.144550916142768e-05</v>
+        <v>-2.18113595418166e-08</v>
       </c>
       <c r="O11" s="3" t="n">
-        <v>-1.694065894508601e-14</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>0.0008774136294534545</v>
+        <v>1.028662655683098e-05</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.0002604481512575462</v>
+        <v>5.244468804480547e-07</v>
       </c>
       <c r="R11" t="n">
-        <v>-0.0002291158765887477</v>
+        <v>-6.921880779308271e-08</v>
       </c>
       <c r="S11" t="n">
-        <v>5.575686668011365e-06</v>
+        <v>3.348108017756841e-07</v>
       </c>
       <c r="T11" t="n">
-        <v>-0.0001403705806935141</v>
+        <v>-1.641283763543079e-06</v>
       </c>
       <c r="U11" t="n">
-        <v>-0.0001227216172633498</v>
+        <v>-2.321662462411632e-06</v>
       </c>
       <c r="V11" t="n">
-        <v>2.990188898896982e-05</v>
+        <v>-3.483238546565528e-06</v>
       </c>
       <c r="W11" t="n">
-        <v>-3.170382206444538e-05</v>
+        <v>-1.887381542969975e-06</v>
       </c>
       <c r="X11" t="n">
-        <v>9.619051760759731e-06</v>
+        <v>3.914576637554622e-10</v>
       </c>
       <c r="Y11" s="4" t="n">
-        <v>0.001926991154014421</v>
+        <v>0.001998941870847453</v>
       </c>
       <c r="Z11" t="n">
-        <v>-0.0001165135081209639</v>
+        <v>1.859421471778613e-06</v>
       </c>
       <c r="AA11" t="n">
-        <v>-1.168512564202087e-06</v>
+        <v>1.056098033490996e-06</v>
       </c>
       <c r="AB11" t="n">
-        <v>-7.747883772410294e-07</v>
+        <v>-2.591444503186033e-10</v>
       </c>
       <c r="AC11" t="n">
-        <v>1.087319770590905e-05</v>
+        <v>3.518633594132334e-07</v>
       </c>
     </row>
     <row r="12">
@@ -1515,88 +1515,88 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>2.100641709190665e-13</v>
+        <v>4.297461776154402e-19</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>-0.03094735254350359</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.004839288106957967</v>
+        <v>3.231174267785264e-21</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>3.263908748184164e-07</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>-3.136744661832878e-08</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>-3.424318203396493e-05</v>
+        <v>1.662620321633785e-09</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>-1.151964808265848e-13</v>
-      </c>
-      <c r="H12" s="2" t="n">
-        <v>-0.001687618378938929</v>
-      </c>
-      <c r="I12" s="2" t="n">
-        <v>-0.00131472331959192</v>
+        <v>-6.196422893331801e-17</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>-9.872059722096694e-09</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>-3.205527506449128e-09</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>0.0001514100072465166</v>
+        <v>-1.092574884499879e-10</v>
       </c>
       <c r="K12" s="3" t="n">
-        <v>8.809142651444724e-14</v>
+        <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.9928108114045417</v>
-      </c>
-      <c r="M12" s="2" t="n">
-        <v>0.001639040830257743</v>
+        <v>0.9999992878965601</v>
+      </c>
+      <c r="M12" s="3" t="n">
+        <v>-3.474728514155879e-07</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>0.0006652387251764079</v>
+        <v>-2.617893891935831e-08</v>
       </c>
       <c r="O12" s="3" t="n">
-        <v>6.776263578034403e-14</v>
+        <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>0.0001039823780058695</v>
-      </c>
-      <c r="Q12" s="4" t="n">
-        <v>-0.001018830163952104</v>
+        <v>1.289817072771415e-08</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-1.133343533970118e-08</v>
       </c>
       <c r="R12" t="n">
-        <v>-0.0008946873294510944</v>
+        <v>9.948253558246019e-09</v>
       </c>
       <c r="S12" t="n">
-        <v>-2.687727013064682e-05</v>
+        <v>-2.806195377237627e-09</v>
       </c>
       <c r="T12" t="n">
-        <v>-1.824532424422138e-05</v>
+        <v>-2.039345674588049e-09</v>
       </c>
       <c r="U12" t="n">
-        <v>6.45986973968663e-05</v>
+        <v>8.542041465911638e-09</v>
       </c>
       <c r="V12" t="n">
-        <v>-0.0001552743567336218</v>
+        <v>9.492112960462328e-09</v>
       </c>
       <c r="W12" t="n">
-        <v>-8.380503498735432e-06</v>
+        <v>4.924098344998081e-09</v>
       </c>
       <c r="X12" t="n">
-        <v>7.483776239772949e-06</v>
+        <v>-1.211633850106228e-12</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.177899918309569e-05</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0.0009445695057147324</v>
+        <v>1.792011796090388e-09</v>
+      </c>
+      <c r="Z12" s="4" t="n">
+        <v>0.001999920903326038</v>
       </c>
       <c r="AA12" t="n">
-        <v>-3.17895612855475e-05</v>
+        <v>-2.056551441791359e-08</v>
       </c>
       <c r="AB12" t="n">
-        <v>3.304680296501838e-05</v>
+        <v>-1.107166483859108e-09</v>
       </c>
       <c r="AC12" t="n">
-        <v>-1.462983215610525e-05</v>
+        <v>-2.176229987012276e-09</v>
       </c>
     </row>
     <row r="13">
@@ -1606,88 +1606,88 @@
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>3.794707603699266e-13</v>
+        <v>0</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D13" s="2" t="n">
-        <v>0.0881753674095891</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>-0.01127794622824536</v>
+      <c r="D13" s="3" t="n">
+        <v>3.463343045051905e-06</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>-8.203946815414664e-07</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>0.0001688777677541411</v>
+        <v>5.214270639045022e-09</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>3.252606517456513e-13</v>
+        <v>-2.729696021424991e-16</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>-0.0001578095707225041</v>
+        <v>-1.591263566207252e-08</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>0.0008391529211684411</v>
+        <v>2.169820031849585e-07</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>-0.000334301437416749</v>
+        <v>-9.702909483510922e-11</v>
       </c>
       <c r="K13" s="3" t="n">
-        <v>-3.523657060577889e-13</v>
+        <v>0</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>0.0006858820312378132</v>
+        <v>-3.059560758880198e-07</v>
       </c>
       <c r="M13" s="2" t="n">
-        <v>0.9897393747841492</v>
-      </c>
-      <c r="N13" s="2" t="n">
-        <v>-0.001190572868699398</v>
+        <v>0.9999968550265748</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>-2.33458911453449e-06</v>
       </c>
       <c r="O13" s="3" t="n">
-        <v>8.131516293641283e-14</v>
+        <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>0.000258912207645734</v>
-      </c>
-      <c r="Q13" s="4" t="n">
-        <v>0.002004738538396349</v>
-      </c>
-      <c r="R13" s="4" t="n">
-        <v>0.002562001546053657</v>
+        <v>1.671929032456526e-08</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1.455641722029696e-07</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1.054961148597646e-07</v>
       </c>
       <c r="S13" t="n">
-        <v>-1.298786328051554e-06</v>
+        <v>-1.2761016110085e-09</v>
       </c>
       <c r="T13" t="n">
-        <v>-3.654125268971915e-05</v>
+        <v>-2.471656978881057e-09</v>
       </c>
       <c r="U13" t="n">
-        <v>1.875881367558938e-05</v>
+        <v>5.607478630211537e-09</v>
       </c>
       <c r="V13" t="n">
-        <v>7.612168341952948e-05</v>
+        <v>5.212243426985989e-09</v>
       </c>
       <c r="W13" t="n">
-        <v>1.920133599645976e-05</v>
+        <v>9.530991670500483e-09</v>
       </c>
       <c r="X13" t="n">
-        <v>-2.178074089359897e-05</v>
+        <v>-2.293704009799316e-12</v>
       </c>
       <c r="Y13" t="n">
-        <v>4.347069037201334e-07</v>
+        <v>1.045498471860668e-09</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.000296969414093377</v>
+        <v>-2.151787339713893e-08</v>
       </c>
       <c r="AA13" s="4" t="n">
-        <v>0.001662809808220629</v>
+        <v>0.001999869072171174</v>
       </c>
       <c r="AB13" t="n">
-        <v>-7.70524151481964e-05</v>
+        <v>-9.857633706838063e-08</v>
       </c>
       <c r="AC13" t="n">
-        <v>-7.312698000307497e-06</v>
+        <v>-1.543499343569996e-09</v>
       </c>
     </row>
     <row r="14">
@@ -1697,88 +1697,88 @@
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>4.87890977618477e-13</v>
+        <v>2.584939414228211e-20</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D14" s="2" t="n">
-        <v>-0.08877877788975422</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.01134281214819951</v>
+      <c r="D14" s="3" t="n">
+        <v>-2.682473495223039e-08</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>1.553283351453764e-09</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>-0.000169966372871649</v>
+        <v>1.712607204807644e-11</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>-9.215718466126788e-13</v>
+        <v>-2.257427590445497e-16</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>0.000174453750138295</v>
+        <v>-6.251472392529953e-11</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>-0.0008367095684651184</v>
+        <v>2.064041141083864e-10</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>0.0003351407221131777</v>
+        <v>-6.757694924246236e-13</v>
       </c>
       <c r="K14" s="3" t="n">
-        <v>-5.963111948670274e-13</v>
+        <v>0</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>-0.0007399770682000369</v>
+        <v>-2.616350380813028e-08</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>0.0004759166667255964</v>
+        <v>-2.333208910938986e-06</v>
       </c>
       <c r="N14" s="2" t="n">
-        <v>0.9918185838369632</v>
+        <v>0.9999978124899631</v>
       </c>
       <c r="O14" s="3" t="n">
-        <v>-4.607859233063394e-13</v>
+        <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>-0.0002598870749680182</v>
-      </c>
-      <c r="Q14" s="4" t="n">
-        <v>-0.002012270912561936</v>
-      </c>
-      <c r="R14" s="4" t="n">
-        <v>-0.002579516506753983</v>
+        <v>3.195981722381248e-10</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>3.371255126063428e-11</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-8.168524956860907e-10</v>
       </c>
       <c r="S14" t="n">
-        <v>1.959954578191828e-06</v>
+        <v>5.27482780294391e-11</v>
       </c>
       <c r="T14" t="n">
-        <v>3.666423721159114e-05</v>
+        <v>-5.250546361964465e-11</v>
       </c>
       <c r="U14" t="n">
-        <v>-1.902702070877803e-05</v>
+        <v>1.005286727326792e-10</v>
       </c>
       <c r="V14" t="n">
-        <v>-7.495273425897099e-05</v>
+        <v>7.181677087633556e-11</v>
       </c>
       <c r="W14" t="n">
-        <v>-1.923162863226406e-05</v>
+        <v>4.413814645783813e-11</v>
       </c>
       <c r="X14" t="n">
-        <v>2.185880941312987e-05</v>
+        <v>-1.0767726688681e-14</v>
       </c>
       <c r="Y14" t="n">
-        <v>-5.013913546500492e-07</v>
+        <v>1.362028329072652e-11</v>
       </c>
       <c r="Z14" t="n">
-        <v>-0.0002940384653967419</v>
+        <v>-1.233377795126003e-09</v>
       </c>
       <c r="AA14" t="n">
-        <v>-7.741335331557138e-05</v>
+        <v>-9.86004944263293e-08</v>
       </c>
       <c r="AB14" s="4" t="n">
-        <v>0.00169038037571307</v>
+        <v>0.001999908919840294</v>
       </c>
       <c r="AC14" t="n">
-        <v>7.394739280543877e-06</v>
+        <v>-2.314133745648719e-11</v>
       </c>
     </row>
     <row r="15">
@@ -1788,88 +1788,88 @@
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>4.065758146820642e-14</v>
+        <v>7.279189390466644e-17</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D15" s="2" t="n">
-        <v>-0.008335147706649206</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0.001344087941040727</v>
+      <c r="D15" s="3" t="n">
+        <v>-2.361791920999475e-06</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>-8.154841151878234e-06</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>-0.0002184211799667883</v>
+        <v>-3.858724074498252e-06</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>4.980553729855286e-13</v>
-      </c>
-      <c r="H15" s="2" t="n">
-        <v>-0.001603803177775744</v>
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="n">
+        <v>-2.063931440041027e-06</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>-0.0009093289684722962</v>
+        <v>2.308790164747859e-06</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>2.144550911738197e-05</v>
+        <v>-2.181135957573101e-08</v>
       </c>
       <c r="K15" s="3" t="n">
-        <v>1.863472483959461e-14</v>
-      </c>
-      <c r="L15" s="2" t="n">
-        <v>0.002061425300144948</v>
-      </c>
-      <c r="M15" s="2" t="n">
-        <v>0.001953138813127266</v>
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>-1.752680562413608e-06</v>
+      </c>
+      <c r="M15" s="3" t="n">
+        <v>-3.857794473757027e-06</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>0.0001207042668093861</v>
+        <v>-6.418436514139038e-09</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>1.000000000000002</v>
+        <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>0.0008774136292637191</v>
+        <v>1.028662655690046e-05</v>
       </c>
       <c r="Q15" t="n">
-        <v>-0.000260448151584501</v>
+        <v>-5.244468804422645e-07</v>
       </c>
       <c r="R15" t="n">
-        <v>-0.0002291158766260171</v>
+        <v>-6.921880793204906e-08</v>
       </c>
       <c r="S15" t="n">
-        <v>-5.575686566367411e-06</v>
+        <v>-3.348108017918141e-07</v>
       </c>
       <c r="T15" t="n">
-        <v>-0.0001403705804953084</v>
+        <v>-1.641283763404113e-06</v>
       </c>
       <c r="U15" t="n">
-        <v>0.0001227216174276742</v>
+        <v>2.321662462446787e-06</v>
       </c>
       <c r="V15" t="n">
-        <v>-0.0001165135081565393</v>
+        <v>1.859421471616072e-06</v>
       </c>
       <c r="W15" t="n">
-        <v>-1.168512886074607e-06</v>
+        <v>1.056098033534009e-06</v>
       </c>
       <c r="X15" t="n">
-        <v>-7.747883060902619e-07</v>
+        <v>-2.591444788563344e-10</v>
       </c>
       <c r="Y15" t="n">
-        <v>1.087319758054817e-05</v>
+        <v>3.518633592970145e-07</v>
       </c>
       <c r="Z15" t="n">
-        <v>2.990188893306565e-05</v>
+        <v>-3.483238546463371e-06</v>
       </c>
       <c r="AA15" t="n">
-        <v>-3.170382204750472e-05</v>
+        <v>-1.88738154294061e-06</v>
       </c>
       <c r="AB15" t="n">
-        <v>9.619051794641049e-06</v>
+        <v>3.914576228100218e-10</v>
       </c>
       <c r="AC15" s="4" t="n">
-        <v>0.001926991154019503</v>
+        <v>0.001998941870847428</v>
       </c>
     </row>
     <row r="16">
@@ -1879,88 +1879,88 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-3.388131789017201e-13</v>
+        <v>-3.252606517456513e-13</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>-0.03962736512571458</v>
+        <v>0.008995250334257587</v>
       </c>
       <c r="E16" t="n">
-        <v>-5.55653613398821e-13</v>
+        <v>4.743384504624082e-14</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>0.008530936315451577</v>
+        <v>0.01513088559289022</v>
       </c>
       <c r="G16" t="n">
-        <v>-2.981555974335137e-13</v>
+        <v>9.656175598699024e-14</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>-0.01065185812256929</v>
+        <v>0.007484292759535837</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>0.001164991514390236</v>
-      </c>
-      <c r="J16" s="4" t="n">
-        <v>0.002569640371389821</v>
+        <v>0.003052568043437453</v>
+      </c>
+      <c r="J16" t="n">
+        <v>6.161277824739964e-05</v>
       </c>
       <c r="K16" t="n">
-        <v>3.523657060577889e-13</v>
+        <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>-0.01065185812469704</v>
+        <v>0.007484292759508732</v>
       </c>
       <c r="M16" s="4" t="n">
-        <v>0.00116499151403787</v>
-      </c>
-      <c r="N16" s="4" t="n">
-        <v>0.00256964037298902</v>
+        <v>0.003052568043393407</v>
+      </c>
+      <c r="N16" t="n">
+        <v>6.161277792722118e-05</v>
       </c>
       <c r="O16" t="n">
-        <v>7.318364664277155e-13</v>
+        <v>0</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0.9994338684510354</v>
+        <v>0.9990094216768499</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>-2.032879073410321e-13</v>
-      </c>
-      <c r="R16" s="2" t="n">
-        <v>-0.001232733441136591</v>
+        <v>-9.825582188149884e-14</v>
+      </c>
+      <c r="R16" s="3" t="n">
+        <v>0.0002709011450950774</v>
       </c>
       <c r="S16" s="3" t="n">
-        <v>-4.336808689942018e-13</v>
+        <v>2.930733997499879e-13</v>
       </c>
       <c r="T16" s="3" t="n">
-        <v>8.800889502575109e-05</v>
+        <v>0.0001585422017363295</v>
       </c>
       <c r="U16" s="3" t="n">
-        <v>-1.897353801849633e-13</v>
-      </c>
-      <c r="V16" s="2" t="n">
-        <v>-0.001916579073330221</v>
+        <v>2.541098841762901e-14</v>
+      </c>
+      <c r="V16" s="3" t="n">
+        <v>7.846525447445421e-05</v>
       </c>
       <c r="W16" s="3" t="n">
-        <v>-4.92077541095013e-05</v>
+        <v>3.192089760648952e-05</v>
       </c>
       <c r="X16" s="3" t="n">
-        <v>0.0001197185468435839</v>
+        <v>6.784913478491764e-09</v>
       </c>
       <c r="Y16" s="3" t="n">
-        <v>1.111207995193805e-05</v>
-      </c>
-      <c r="Z16" s="2" t="n">
-        <v>-0.001916579073289564</v>
+        <v>1.479065061074127e-05</v>
+      </c>
+      <c r="Z16" s="3" t="n">
+        <v>7.846525438975091e-05</v>
       </c>
       <c r="AA16" s="3" t="n">
-        <v>-4.920775385200329e-05</v>
+        <v>3.192089800120688e-05</v>
       </c>
       <c r="AB16" s="3" t="n">
-        <v>0.0001197185467216111</v>
+        <v>6.784700026189056e-09</v>
       </c>
       <c r="AC16" s="3" t="n">
-        <v>1.111208016877849e-05</v>
+        <v>1.479065058363621e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1970,88 +1970,88 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.41587469199985e-12</v>
+        <v>1.609754756874604e-15</v>
       </c>
       <c r="C17" t="n">
-        <v>-1.638581061568252e-14</v>
+        <v>-3.016470643570088e-15</v>
       </c>
       <c r="D17" t="n">
-        <v>1.012583013750502e-12</v>
+        <v>1.527942929742011e-13</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0.280055297953877</v>
+        <v>0.7447332426266492</v>
       </c>
       <c r="F17" t="n">
-        <v>-2.553900462647902e-13</v>
+        <v>4.210729867639096e-14</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0002023041279821564</v>
+        <v>-2.759531321485623e-05</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>-0.006201967762399277</v>
+        <v>0.01379130720283105</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>-0.0561130465937454</v>
-      </c>
-      <c r="J17" s="4" t="n">
-        <v>0.01729155721933702</v>
+        <v>-0.2823533455306256</v>
+      </c>
+      <c r="J17" t="n">
+        <v>4.895975753650296e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>-1.423579957681027e-13</v>
+        <v>7.634049261810735e-24</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>0.006201967761862126</v>
+        <v>-0.01379130720269334</v>
       </c>
       <c r="M17" s="4" t="n">
-        <v>0.05611304659538683</v>
-      </c>
-      <c r="N17" s="4" t="n">
-        <v>-0.01729155721410868</v>
+        <v>0.282353345530324</v>
+      </c>
+      <c r="N17" t="n">
+        <v>-4.895975673850405e-05</v>
       </c>
       <c r="O17" t="n">
-        <v>-3.564174373804528e-12</v>
+        <v>7.634097410059345e-24</v>
       </c>
       <c r="P17" s="3" t="n">
-        <v>1.03042579082794e-12</v>
+        <v>-3.06238491618816e-13</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>0.9510813374823789</v>
+        <v>0.8597752649709076</v>
       </c>
       <c r="R17" s="3" t="n">
-        <v>-8.209264697592001e-13</v>
+        <v>3.291327533222199e-14</v>
       </c>
       <c r="S17" s="3" t="n">
-        <v>0.0004849181336699154</v>
+        <v>0.000436506099918696</v>
       </c>
       <c r="T17" s="3" t="n">
-        <v>-2.703322833774428e-12</v>
+        <v>3.927874835521808e-13</v>
       </c>
       <c r="U17" s="3" t="n">
-        <v>0.0007050214672528791</v>
-      </c>
-      <c r="V17" s="2" t="n">
-        <v>-0.00482452920307939</v>
+        <v>2.881032600004228e-05</v>
+      </c>
+      <c r="V17" s="3" t="n">
+        <v>0.000195990294312499</v>
       </c>
       <c r="W17" s="2" t="n">
-        <v>-0.001052558787975825</v>
-      </c>
-      <c r="X17" s="2" t="n">
-        <v>0.001110594485744903</v>
+        <v>-0.008714923243773331</v>
+      </c>
+      <c r="X17" s="3" t="n">
+        <v>2.066969931919369e-06</v>
       </c>
       <c r="Y17" s="3" t="n">
-        <v>0.0001038513042712877</v>
-      </c>
-      <c r="Z17" s="2" t="n">
-        <v>0.004824529205827433</v>
+        <v>-4.23990265632638e-05</v>
+      </c>
+      <c r="Z17" s="3" t="n">
+        <v>-0.0001959902934995039</v>
       </c>
       <c r="AA17" s="2" t="n">
-        <v>0.001052558789642329</v>
-      </c>
-      <c r="AB17" s="2" t="n">
-        <v>-0.001110594487541579</v>
+        <v>0.008714923243530927</v>
+      </c>
+      <c r="AB17" s="3" t="n">
+        <v>-2.06697031265664e-06</v>
       </c>
       <c r="AC17" s="3" t="n">
-        <v>-0.0001038513025223567</v>
+        <v>4.239902697984923e-05</v>
       </c>
     </row>
     <row r="18">
@@ -2061,88 +2061,88 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>1.641126335305207e-14</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>-3.94137541592874</v>
+        <v>-6.316815300650524</v>
       </c>
       <c r="E18" t="n">
-        <v>-6.938893903907228e-12</v>
+        <v>-3.398613821739473e-12</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>-0.009138092334042003</v>
+        <v>-0.01190378934007634</v>
       </c>
       <c r="G18" t="n">
-        <v>-1.734723475976807e-12</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.0008546500330358642</v>
+        <v>-7.30565917006834e-15</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>-0.009553995601310029</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>0.06541581910358973</v>
-      </c>
-      <c r="J18" s="4" t="n">
-        <v>-0.02226369937800149</v>
+        <v>0.1934789676691003</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-3.452787962390781e-05</v>
       </c>
       <c r="K18" t="n">
-        <v>-4.336808689942018e-12</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0.000854650030433779</v>
+        <v>0</v>
+      </c>
+      <c r="L18" s="4" t="n">
+        <v>-0.009553995601308228</v>
       </c>
       <c r="M18" s="4" t="n">
-        <v>0.06541581911486544</v>
-      </c>
-      <c r="N18" s="4" t="n">
-        <v>-0.02226369937192996</v>
+        <v>0.193478967667414</v>
+      </c>
+      <c r="N18" t="n">
+        <v>-3.452787621227085e-05</v>
       </c>
       <c r="O18" t="n">
-        <v>-5.204170427930421e-12</v>
+        <v>0</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>0.005114093004111864</v>
+        <v>-0.002378830216249672</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>6.938893903907228e-12</v>
+        <v>7.199780051661553e-15</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>0.8857800666024068</v>
+        <v>0.8075970466333712</v>
       </c>
       <c r="S18" s="3" t="n">
-        <v>-4.336808689942018e-12</v>
-      </c>
-      <c r="T18" s="2" t="n">
-        <v>-0.001027657860717957</v>
+        <v>-5.115020210231906e-12</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>2.245857666600493e-05</v>
       </c>
       <c r="U18" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" s="2" t="n">
-        <v>0.005785221012313824</v>
+        <v>-1.699465729547347e-12</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>-0.0001005734736349581</v>
       </c>
       <c r="W18" s="2" t="n">
-        <v>0.001322842245465861</v>
-      </c>
-      <c r="X18" s="2" t="n">
-        <v>-0.001436897191509079</v>
+        <v>0.005990563748253547</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>-1.42238200230031e-06</v>
       </c>
       <c r="Y18" s="3" t="n">
-        <v>-6.732082166033271e-05</v>
-      </c>
-      <c r="Z18" s="2" t="n">
-        <v>0.005785221014048547</v>
+        <v>3.54310710845816e-05</v>
+      </c>
+      <c r="Z18" s="3" t="n">
+        <v>-0.0001005734770473362</v>
       </c>
       <c r="AA18" s="2" t="n">
-        <v>0.001322842243731137</v>
-      </c>
-      <c r="AB18" s="2" t="n">
-        <v>-0.00143689718717227</v>
+        <v>0.00599056374483651</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>-1.422383675508018e-06</v>
       </c>
       <c r="AC18" s="3" t="n">
-        <v>-6.73208147214388e-05</v>
+        <v>3.543106938098659e-05</v>
       </c>
     </row>
     <row r="19">
@@ -2152,88 +2152,88 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-1.046104161547901e-12</v>
+        <v>-2.233950180693945e-13</v>
       </c>
       <c r="C19" t="n">
-        <v>6.2257467680671e-13</v>
+        <v>1.13813954650278e-13</v>
       </c>
       <c r="D19" t="n">
-        <v>-5.36088954614e-11</v>
+        <v>-9.303700511342585e-12</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>-2.054977058406312</v>
+        <v>-5.378075886090482</v>
       </c>
       <c r="F19" t="n">
-        <v>-6.233143369316087e-11</v>
+        <v>-6.339295199505375e-12</v>
       </c>
       <c r="G19" t="n">
-        <v>7.708077589534431e-11</v>
+        <v>-9.421011138213063e-12</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0.07215812925749741</v>
+        <v>-0.0995883049336521</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>0.4393531579744172</v>
-      </c>
-      <c r="J19" s="4" t="n">
-        <v>-0.128669869558497</v>
+        <v>2.039020697434511</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-0.0003460374474030068</v>
       </c>
       <c r="K19" t="n">
-        <v>5.888884972058033e-11</v>
+        <v>-2.893825297238485e-22</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>-0.07215812928939579</v>
+        <v>0.0995883049325231</v>
       </c>
       <c r="M19" s="4" t="n">
-        <v>-0.4393531579890865</v>
-      </c>
-      <c r="N19" s="4" t="n">
-        <v>0.1286698695555051</v>
+        <v>-2.039020697410847</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.0003460374052088849</v>
       </c>
       <c r="O19" t="n">
-        <v>7.845577099042248e-11</v>
+        <v>-2.893886926996705e-22</v>
       </c>
       <c r="P19" s="3" t="n">
-        <v>-9.262822690384554e-11</v>
+        <v>1.129949280004955e-11</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>-0.9038308290246734</v>
+        <v>-0.266674972214326</v>
       </c>
       <c r="R19" s="3" t="n">
-        <v>-4.454310681470254e-12</v>
+        <v>-9.358881839883531e-13</v>
       </c>
       <c r="S19" s="2" t="n">
-        <v>0.7934433219352142</v>
+        <v>0.7927455305447909</v>
       </c>
       <c r="T19" s="3" t="n">
-        <v>9.007831199767673e-11</v>
-      </c>
-      <c r="U19" s="2" t="n">
-        <v>-0.004356515159313379</v>
+        <v>-1.522182343022594e-11</v>
+      </c>
+      <c r="U19" s="3" t="n">
+        <v>-0.0004557900037285972</v>
       </c>
       <c r="V19" s="2" t="n">
-        <v>0.03770209209643688</v>
+        <v>-0.003960640509688269</v>
       </c>
       <c r="W19" s="2" t="n">
-        <v>0.008013552761212205</v>
-      </c>
-      <c r="X19" s="2" t="n">
-        <v>-0.00822471402494975</v>
+        <v>0.0616242723074032</v>
+      </c>
+      <c r="X19" s="3" t="n">
+        <v>-1.460882610826533e-05</v>
       </c>
       <c r="Y19" s="3" t="n">
-        <v>-0.0009761397026352427</v>
+        <v>-0.0001742674560975501</v>
       </c>
       <c r="Z19" s="2" t="n">
-        <v>-0.0377020923580837</v>
+        <v>0.003960640471671464</v>
       </c>
       <c r="AA19" s="2" t="n">
-        <v>-0.008013552658890328</v>
-      </c>
-      <c r="AB19" s="2" t="n">
-        <v>0.008224714145058053</v>
+        <v>-0.06162427230625438</v>
+      </c>
+      <c r="AB19" s="3" t="n">
+        <v>1.460883291837654e-05</v>
       </c>
       <c r="AC19" s="3" t="n">
-        <v>0.0009761396515054184</v>
+        <v>0.0001742674490997075</v>
       </c>
     </row>
     <row r="20">
@@ -2243,88 +2243,88 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-1.275021754842953e-10</v>
+        <v>-8.077306185017008e-12</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>-7.376196588247327</v>
+        <v>0.04120607686926855</v>
       </c>
       <c r="E20" t="n">
-        <v>8.239936510889834e-11</v>
+        <v>1.870248747537495e-12</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0.1116576653151236</v>
+        <v>0.1095530478601342</v>
       </c>
       <c r="G20" t="n">
-        <v>1.058181320345852e-10</v>
+        <v>3.618524750670371e-12</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>2.060709051962019</v>
+        <v>0.05439413020204992</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>1.107142004064081</v>
+        <v>0.02330434828681674</v>
       </c>
       <c r="J20" t="n">
-        <v>-0.0008246133055903049</v>
+        <v>0.0007443602157585936</v>
       </c>
       <c r="K20" t="n">
-        <v>3.295974604355933e-11</v>
+        <v>0</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>2.060709052196207</v>
+        <v>0.05439413020112834</v>
       </c>
       <c r="M20" s="4" t="n">
-        <v>1.107142003980814</v>
+        <v>0.02330434828128731</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.0008246134278883099</v>
+        <v>0.0007443602076677349</v>
       </c>
       <c r="O20" t="n">
-        <v>-3.816391647148976e-11</v>
+        <v>0</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>1.068844712364195</v>
+        <v>1.270983418775808</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>-1.110223024625157e-10</v>
+        <v>-3.63207727782644e-12</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>-0.1894243574253329</v>
+        <v>0.001930917343457629</v>
       </c>
       <c r="S20" s="3" t="n">
-        <v>5.204170427930421e-12</v>
+        <v>1.09910995235718e-11</v>
       </c>
       <c r="T20" s="2" t="n">
-        <v>0.8291702785993144</v>
+        <v>0.7972275645696316</v>
       </c>
       <c r="U20" s="3" t="n">
-        <v>5.204170427930421e-11</v>
+        <v>9.486769009248164e-13</v>
       </c>
       <c r="V20" s="2" t="n">
-        <v>0.1427312421404744</v>
-      </c>
-      <c r="W20" s="3" t="n">
-        <v>-0.0005698265323136886</v>
-      </c>
-      <c r="X20" s="2" t="n">
-        <v>0.002757954897444903</v>
+        <v>-0.1002885938598445</v>
+      </c>
+      <c r="W20" s="2" t="n">
+        <v>-0.05166923530788056</v>
+      </c>
+      <c r="X20" s="3" t="n">
+        <v>1.263296601659511e-05</v>
       </c>
       <c r="Y20" s="2" t="n">
-        <v>-0.01441044807527075</v>
+        <v>-0.01893044018907324</v>
       </c>
       <c r="Z20" s="2" t="n">
-        <v>0.1427312421595564</v>
-      </c>
-      <c r="AA20" s="3" t="n">
-        <v>-0.0005698263536371706</v>
-      </c>
-      <c r="AB20" s="2" t="n">
-        <v>0.002757954921731032</v>
+        <v>-0.1002885938511844</v>
+      </c>
+      <c r="AA20" s="2" t="n">
+        <v>-0.0516692352970792</v>
+      </c>
+      <c r="AB20" s="3" t="n">
+        <v>1.263295414458132e-05</v>
       </c>
       <c r="AC20" s="2" t="n">
-        <v>-0.01441044800935126</v>
+        <v>-0.018930440186173</v>
       </c>
     </row>
     <row r="21">
@@ -2334,88 +2334,88 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-2.17377831832724e-11</v>
+        <v>-2.142121267987094e-12</v>
       </c>
       <c r="C21" t="n">
-        <v>1.473193212143807e-13</v>
+        <v>1.667972467202707e-14</v>
       </c>
       <c r="D21" t="n">
-        <v>2.599299420621617e-11</v>
+        <v>4.658335035663008e-12</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>-0.7659004995612656</v>
+        <v>-0.06724764714273139</v>
       </c>
       <c r="F21" t="n">
-        <v>-8.01427458635015e-12</v>
+        <v>-1.062352181193065e-11</v>
       </c>
       <c r="G21" t="n">
-        <v>-3.12408736179312e-10</v>
-      </c>
-      <c r="H21" s="4" t="n">
-        <v>2.04287840233373</v>
+        <v>4.190231663692277e-13</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-0.0008540808986943678</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>1.063836068585355</v>
-      </c>
-      <c r="J21" s="4" t="n">
-        <v>-0.04959924620071828</v>
+        <v>0.0263788188205093</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0005482514726446857</v>
       </c>
       <c r="K21" t="n">
-        <v>1.849519512963067e-12</v>
-      </c>
-      <c r="L21" s="4" t="n">
-        <v>-2.042878402314091</v>
+        <v>-5.983016928035611e-23</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.000854080899361205</v>
       </c>
       <c r="M21" s="4" t="n">
-        <v>-1.063836068675396</v>
-      </c>
-      <c r="N21" s="4" t="n">
-        <v>0.04959924617604131</v>
+        <v>-0.02637881881349029</v>
+      </c>
+      <c r="N21" t="n">
+        <v>-0.0005482514798135377</v>
       </c>
       <c r="O21" t="n">
-        <v>-1.421891531577611e-11</v>
+        <v>-5.983093965233387e-23</v>
       </c>
       <c r="P21" s="3" t="n">
-        <v>-9.800642785823241e-12</v>
+        <v>-1.652759349725905e-12</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>-0.05661566082530929</v>
+        <v>-0.00399473445328697</v>
       </c>
       <c r="R21" s="3" t="n">
-        <v>7.107517838543248e-12</v>
+        <v>3.830567223485151e-12</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>-0.02899315813965262</v>
+        <v>-0.002593904369716818</v>
       </c>
       <c r="T21" s="3" t="n">
-        <v>-1.160476181816457e-11</v>
+        <v>-7.439149517573695e-12</v>
       </c>
       <c r="U21" s="2" t="n">
-        <v>0.8986436853625002</v>
+        <v>0.8074480278491321</v>
       </c>
       <c r="V21" s="2" t="n">
-        <v>0.1619802833217399</v>
-      </c>
-      <c r="W21" s="3" t="n">
-        <v>0.0008481410569004863</v>
+        <v>-0.1869715098309358</v>
+      </c>
+      <c r="W21" s="2" t="n">
+        <v>-0.09545979642644954</v>
       </c>
       <c r="X21" s="3" t="n">
-        <v>8.264374355147619e-06</v>
+        <v>2.315005318370776e-05</v>
       </c>
       <c r="Y21" s="2" t="n">
-        <v>-0.01386867522694637</v>
+        <v>-0.03528558425645998</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>-0.1619802833580427</v>
-      </c>
-      <c r="AA21" s="3" t="n">
-        <v>-0.0008481409760179219</v>
+        <v>0.1869715098339775</v>
+      </c>
+      <c r="AA21" s="2" t="n">
+        <v>0.09545979642673125</v>
       </c>
       <c r="AB21" s="3" t="n">
-        <v>-8.264379087004781e-06</v>
+        <v>-2.315004634260431e-05</v>
       </c>
       <c r="AC21" s="2" t="n">
-        <v>0.01386867523045432</v>
+        <v>0.0352855842646974</v>
       </c>
     </row>
     <row r="22">
@@ -2425,88 +2425,88 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-8.673617379884035e-11</v>
+        <v>1.174596469825299e-16</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>-15.47367627181134</v>
-      </c>
-      <c r="E22" s="4" t="n">
-        <v>-2.419644053636843</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>-0.01712159117261969</v>
+        <v>-1.654361225106055e-18</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0001631954374096475</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.568372330940045e-05</v>
+      </c>
+      <c r="F22" t="n">
+        <v>8.313101604698646e-07</v>
       </c>
       <c r="G22" t="n">
-        <v>-4.163336342344337e-11</v>
-      </c>
-      <c r="H22" s="4" t="n">
-        <v>-3.594594297509635</v>
-      </c>
-      <c r="I22" s="4" t="n">
-        <v>0.8195204151267843</v>
-      </c>
-      <c r="J22" s="4" t="n">
-        <v>0.3326193624558771</v>
+        <v>3.043032037460078e-14</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.0003560517199515963</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-0.000173736425707914</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-1.308946945963012e-05</v>
       </c>
       <c r="K22" t="n">
-        <v>9.71445146547012e-11</v>
-      </c>
-      <c r="L22" s="4" t="n">
-        <v>-0.8438091898405053</v>
-      </c>
-      <c r="M22" s="4" t="n">
-        <v>-0.6573616597310705</v>
-      </c>
-      <c r="N22" s="4" t="n">
-        <v>0.07570500382136913</v>
+        <v>0</v>
+      </c>
+      <c r="L22" t="n">
+        <v>-4.936029860867891e-06</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-1.602763753188478e-06</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-5.462874402256734e-08</v>
       </c>
       <c r="O22" t="n">
-        <v>9.367506770274758e-11</v>
-      </c>
-      <c r="P22" s="2" t="n">
-        <v>0.05199118923229773</v>
-      </c>
-      <c r="Q22" s="2" t="n">
-        <v>0.5094150818153731</v>
-      </c>
-      <c r="R22" s="2" t="n">
-        <v>-0.4473436646980355</v>
-      </c>
-      <c r="S22" s="2" t="n">
-        <v>0.01343863501729325</v>
-      </c>
-      <c r="T22" s="2" t="n">
-        <v>-0.009122662309596352</v>
-      </c>
-      <c r="U22" s="2" t="n">
-        <v>-0.03229934864359962</v>
+        <v>0</v>
+      </c>
+      <c r="P22" s="3" t="n">
+        <v>6.449085363554638e-06</v>
+      </c>
+      <c r="Q22" s="3" t="n">
+        <v>5.66671766994586e-06</v>
+      </c>
+      <c r="R22" s="3" t="n">
+        <v>4.974126779329507e-06</v>
+      </c>
+      <c r="S22" s="3" t="n">
+        <v>1.403097688675979e-06</v>
+      </c>
+      <c r="T22" s="3" t="n">
+        <v>-1.019672837488864e-06</v>
+      </c>
+      <c r="U22" s="3" t="n">
+        <v>-4.271020732803876e-06</v>
       </c>
       <c r="V22" s="2" t="n">
-        <v>0.4722847529309293</v>
-      </c>
-      <c r="W22" s="2" t="n">
-        <v>-0.01589478061322924</v>
-      </c>
-      <c r="X22" s="2" t="n">
-        <v>0.01652340141794495</v>
-      </c>
-      <c r="Y22" s="2" t="n">
-        <v>-0.00731491603747636</v>
-      </c>
-      <c r="Z22" s="2" t="n">
-        <v>-0.07763717836672956</v>
-      </c>
-      <c r="AA22" s="2" t="n">
-        <v>-0.004190251562397052</v>
-      </c>
-      <c r="AB22" s="2" t="n">
-        <v>0.003741888056352227</v>
-      </c>
-      <c r="AC22" s="2" t="n">
-        <v>0.005889499669203824</v>
+        <v>0.9999604516630191</v>
+      </c>
+      <c r="W22" s="3" t="n">
+        <v>-1.028275720897141e-05</v>
+      </c>
+      <c r="X22" s="3" t="n">
+        <v>-5.535832421259187e-07</v>
+      </c>
+      <c r="Y22" s="3" t="n">
+        <v>-1.088114993480185e-06</v>
+      </c>
+      <c r="Z22" s="3" t="n">
+        <v>4.746056480940238e-06</v>
+      </c>
+      <c r="AA22" s="3" t="n">
+        <v>2.462049172365929e-06</v>
+      </c>
+      <c r="AB22" s="3" t="n">
+        <v>-6.058166184534499e-10</v>
+      </c>
+      <c r="AC22" s="3" t="n">
+        <v>8.960058981412892e-07</v>
       </c>
     </row>
     <row r="23">
@@ -2516,88 +2516,88 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3.747002708109903e-10</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>44.08768370445237</v>
-      </c>
-      <c r="E23" s="4" t="n">
-        <v>5.638973114369117</v>
-      </c>
-      <c r="F23" s="4" t="n">
-        <v>0.08443888421805212</v>
+        <v>0.001731671522527984</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0004101973407728574</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2.607135318417398e-06</v>
       </c>
       <c r="G23" t="n">
-        <v>1.52655665885959e-10</v>
-      </c>
-      <c r="H23" s="4" t="n">
-        <v>0.3429410153077406</v>
+        <v>1.363723045079424e-13</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-0.0001529780379444433</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>-5.13031260793162</v>
+        <v>-0.001572486712709243</v>
       </c>
       <c r="J23" s="4" t="n">
-        <v>-0.5952864338548691</v>
+        <v>-0.001167294557267033</v>
       </c>
       <c r="K23" t="n">
-        <v>1.387778780781446e-10</v>
-      </c>
-      <c r="L23" s="4" t="n">
-        <v>-0.07890478553873592</v>
-      </c>
-      <c r="M23" s="4" t="n">
-        <v>0.4195764607278774</v>
-      </c>
-      <c r="N23" s="4" t="n">
-        <v>-0.1671507182249288</v>
+        <v>0</v>
+      </c>
+      <c r="L23" t="n">
+        <v>-7.956317831810502e-06</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.0001084910015917844</v>
+      </c>
+      <c r="N23" t="n">
+        <v>-4.851454770210474e-08</v>
       </c>
       <c r="O23" t="n">
-        <v>-8.326672684688674e-11</v>
-      </c>
-      <c r="P23" s="2" t="n">
-        <v>0.1294561041281783</v>
-      </c>
-      <c r="Q23" s="2" t="n">
-        <v>-1.002369269559322</v>
-      </c>
-      <c r="R23" s="2" t="n">
-        <v>1.281000773040164</v>
+        <v>0</v>
+      </c>
+      <c r="P23" s="3" t="n">
+        <v>8.359645162060947e-06</v>
+      </c>
+      <c r="Q23" s="3" t="n">
+        <v>-7.278208610127633e-05</v>
+      </c>
+      <c r="R23" s="3" t="n">
+        <v>5.274805743001797e-05</v>
       </c>
       <c r="S23" s="3" t="n">
-        <v>0.0006493939969098861</v>
-      </c>
-      <c r="T23" s="2" t="n">
-        <v>-0.01827062635906262</v>
-      </c>
-      <c r="U23" s="2" t="n">
-        <v>-0.009379406515352962</v>
-      </c>
-      <c r="V23" s="2" t="n">
-        <v>0.1484847073490725</v>
+        <v>6.380508050211767e-07</v>
+      </c>
+      <c r="T23" s="3" t="n">
+        <v>-1.235828489629126e-06</v>
+      </c>
+      <c r="U23" s="3" t="n">
+        <v>-2.803739315876701e-06</v>
+      </c>
+      <c r="V23" s="3" t="n">
+        <v>-1.07589366984338e-05</v>
       </c>
       <c r="W23" s="2" t="n">
-        <v>0.8314049042834615</v>
-      </c>
-      <c r="X23" s="2" t="n">
-        <v>-0.03852620726607636</v>
-      </c>
-      <c r="Y23" s="2" t="n">
-        <v>-0.003656348973590795</v>
-      </c>
-      <c r="Z23" s="2" t="n">
-        <v>0.03806084186708247</v>
-      </c>
-      <c r="AA23" s="2" t="n">
-        <v>0.00960066785793412</v>
-      </c>
-      <c r="AB23" s="2" t="n">
-        <v>-0.01089037068857657</v>
+        <v>0.9999345360855875</v>
+      </c>
+      <c r="X23" s="3" t="n">
+        <v>-4.928816853421347e-05</v>
+      </c>
+      <c r="Y23" s="3" t="n">
+        <v>-7.717496723772595e-07</v>
+      </c>
+      <c r="Z23" s="3" t="n">
+        <v>2.606121714323484e-06</v>
+      </c>
+      <c r="AA23" s="3" t="n">
+        <v>4.765495834691067e-06</v>
+      </c>
+      <c r="AB23" s="3" t="n">
+        <v>-1.146852117396222e-09</v>
       </c>
       <c r="AC23" s="3" t="n">
-        <v>0.0002173535101901436</v>
+        <v>5.227492357814413e-07</v>
       </c>
     </row>
     <row r="24">
@@ -2607,88 +2607,88 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.024558464266192e-10</v>
+        <v>1.323488980084844e-17</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="4" t="n">
-        <v>-44.38938894521516</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>-5.67140607421468</v>
-      </c>
-      <c r="F24" s="4" t="n">
-        <v>-0.08498318601612986</v>
+      <c r="D24" t="n">
+        <v>-1.341236747611589e-05</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-7.766416757475616e-07</v>
+      </c>
+      <c r="F24" t="n">
+        <v>8.56303601762757e-09</v>
       </c>
       <c r="G24" t="n">
-        <v>6.38378239159465e-10</v>
-      </c>
-      <c r="H24" s="4" t="n">
-        <v>-0.3699885342822729</v>
+        <v>1.128704489440857e-13</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-1.308175190406747e-05</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>0.2379583330242019</v>
+        <v>-0.001166604455469484</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>-4.090708081397332</v>
+        <v>-0.001093755018411609</v>
       </c>
       <c r="K24" t="n">
-        <v>-8.326672684688674e-11</v>
-      </c>
-      <c r="L24" s="4" t="n">
-        <v>0.08722687495910098</v>
-      </c>
-      <c r="M24" s="4" t="n">
-        <v>-0.4183547839681223</v>
-      </c>
-      <c r="N24" s="4" t="n">
-        <v>0.1675703613784885</v>
+        <v>0</v>
+      </c>
+      <c r="L24" t="n">
+        <v>-3.12573619612539e-08</v>
+      </c>
+      <c r="M24" t="n">
+        <v>1.032020570557183e-07</v>
+      </c>
+      <c r="N24" t="n">
+        <v>-3.378847381473008e-10</v>
       </c>
       <c r="O24" t="n">
-        <v>-8.326672684688674e-11</v>
-      </c>
-      <c r="P24" s="2" t="n">
-        <v>-0.1299435374024771</v>
-      </c>
-      <c r="Q24" s="2" t="n">
-        <v>1.006135456435575</v>
-      </c>
-      <c r="R24" s="2" t="n">
-        <v>-1.289758253364415</v>
+        <v>0</v>
+      </c>
+      <c r="P24" s="3" t="n">
+        <v>1.597990861189332e-07</v>
+      </c>
+      <c r="Q24" s="3" t="n">
+        <v>-1.685627563029129e-08</v>
+      </c>
+      <c r="R24" s="3" t="n">
+        <v>-4.084262478415719e-07</v>
       </c>
       <c r="S24" s="3" t="n">
-        <v>-0.0009799767802798343</v>
-      </c>
-      <c r="T24" s="2" t="n">
-        <v>0.01833211885071684</v>
-      </c>
-      <c r="U24" s="2" t="n">
-        <v>0.009513510437764161</v>
-      </c>
-      <c r="V24" s="2" t="n">
-        <v>-0.1470192325103703</v>
-      </c>
-      <c r="W24" s="2" t="n">
-        <v>-0.03870667664163108</v>
+        <v>-2.637413903043598e-08</v>
+      </c>
+      <c r="T24" s="3" t="n">
+        <v>-2.625273180956383e-08</v>
+      </c>
+      <c r="U24" s="3" t="n">
+        <v>-5.026433637373252e-08</v>
+      </c>
+      <c r="V24" s="3" t="n">
+        <v>-6.166888975583745e-07</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <v>-4.930024721315893e-05</v>
       </c>
       <c r="X24" s="2" t="n">
-        <v>0.8451901881284529</v>
-      </c>
-      <c r="Y24" s="2" t="n">
-        <v>0.003697369521660221</v>
-      </c>
-      <c r="Z24" s="2" t="n">
-        <v>-0.03747636700968116</v>
-      </c>
-      <c r="AA24" s="2" t="n">
-        <v>-0.009615814769436959</v>
-      </c>
-      <c r="AB24" s="2" t="n">
-        <v>0.01092940471458803</v>
+        <v>0.9999544599201468</v>
+      </c>
+      <c r="Y24" s="3" t="n">
+        <v>-1.157066872511582e-08</v>
+      </c>
+      <c r="Z24" s="3" t="n">
+        <v>3.590838543413528e-08</v>
+      </c>
+      <c r="AA24" s="3" t="n">
+        <v>2.20690732211384e-08</v>
+      </c>
+      <c r="AB24" s="3" t="n">
+        <v>-5.383860526756541e-12</v>
       </c>
       <c r="AC24" s="3" t="n">
-        <v>-0.0002506956864323229</v>
+        <v>6.810141640141684e-09</v>
       </c>
     </row>
     <row r="25">
@@ -2698,88 +2698,88 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-5.551115123125783e-11</v>
+        <v>1.905824131322176e-15</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>-4.167573853319263</v>
+        <v>-0.001180895960398704</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>-0.6720439704897483</v>
+        <v>0.004077420575916473</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>-0.1092105900071111</v>
+        <v>-0.001929362037352174</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.786765180256111e-10</v>
-      </c>
-      <c r="H25" s="4" t="n">
-        <v>1.030712650031823</v>
+        <v>-1.058791184067875e-15</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-0.0008763402812149417</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>0.9765694065442393</v>
-      </c>
-      <c r="J25" s="4" t="n">
-        <v>0.06035213343403428</v>
+        <v>-0.001928897236866451</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-3.209218276466904e-06</v>
       </c>
       <c r="K25" t="n">
-        <v>4.510281037539698e-11</v>
+        <v>0</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>-0.8019015888989511</v>
+        <v>-0.001031965720002448</v>
       </c>
       <c r="M25" s="4" t="n">
-        <v>-0.454664484273587</v>
-      </c>
-      <c r="N25" s="4" t="n">
-        <v>0.01072275458008365</v>
+        <v>0.00115439508233535</v>
+      </c>
+      <c r="N25" t="n">
+        <v>-1.090567977089838e-05</v>
       </c>
       <c r="O25" t="n">
-        <v>-8.673617379884035e-12</v>
+        <v>0</v>
       </c>
       <c r="P25" s="2" t="n">
-        <v>0.4387068147267137</v>
-      </c>
-      <c r="Q25" s="2" t="n">
-        <v>0.130224075628807</v>
-      </c>
-      <c r="R25" s="2" t="n">
-        <v>-0.1145579382943671</v>
-      </c>
-      <c r="S25" s="2" t="n">
-        <v>0.002787843333788842</v>
-      </c>
-      <c r="T25" s="2" t="n">
-        <v>-0.07018529034688581</v>
+        <v>0.005143313278415341</v>
+      </c>
+      <c r="Q25" s="3" t="n">
+        <v>0.0002622234402240869</v>
+      </c>
+      <c r="R25" s="3" t="n">
+        <v>-3.460940389651489e-05</v>
+      </c>
+      <c r="S25" s="3" t="n">
+        <v>0.0001674054008878205</v>
+      </c>
+      <c r="T25" s="3" t="n">
+        <v>-0.0008206418817715412</v>
       </c>
       <c r="U25" s="2" t="n">
-        <v>-0.0613608086312209</v>
+        <v>-0.001160831231205678</v>
       </c>
       <c r="V25" s="2" t="n">
-        <v>0.01495094449459333</v>
-      </c>
-      <c r="W25" s="2" t="n">
-        <v>-0.01585191103208039</v>
-      </c>
-      <c r="X25" s="2" t="n">
-        <v>0.004809525879986842</v>
+        <v>-0.001741619273282909</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <v>-0.0009436907714851776</v>
+      </c>
+      <c r="X25" s="3" t="n">
+        <v>1.957288320067713e-07</v>
       </c>
       <c r="Y25" s="2" t="n">
-        <v>0.963495577007041</v>
-      </c>
-      <c r="Z25" s="2" t="n">
-        <v>-0.0582567540605497</v>
+        <v>0.9994709354237266</v>
+      </c>
+      <c r="Z25" s="3" t="n">
+        <v>0.0009297107358893628</v>
       </c>
       <c r="AA25" s="3" t="n">
-        <v>-0.000584256282243345</v>
+        <v>0.0005280490167454532</v>
       </c>
       <c r="AB25" s="3" t="n">
-        <v>-0.0003873941887763688</v>
-      </c>
-      <c r="AC25" s="2" t="n">
-        <v>0.005436598853394981</v>
+        <v>-1.295722251162882e-07</v>
+      </c>
+      <c r="AC25" s="3" t="n">
+        <v>0.0001759316797067259</v>
       </c>
     </row>
     <row r="26">
@@ -2789,88 +2789,88 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.040834085586084e-10</v>
+        <v>2.150669592637872e-16</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>-15.47367627174889</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>2.419644053480718</v>
-      </c>
-      <c r="F26" s="4" t="n">
-        <v>-0.01712159101996402</v>
+        <v>1.654361225106055e-18</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0001631954374092074</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-1.568372330916387e-05</v>
+      </c>
+      <c r="F26" t="n">
+        <v>8.313101608172805e-07</v>
       </c>
       <c r="G26" t="n">
-        <v>-5.898059818321144e-11</v>
-      </c>
-      <c r="H26" s="4" t="n">
-        <v>-0.8438091894692745</v>
-      </c>
-      <c r="I26" s="4" t="n">
-        <v>-0.65736165979699</v>
-      </c>
-      <c r="J26" s="4" t="n">
-        <v>0.07570500362361066</v>
+        <v>-3.09812226625611e-14</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-4.936029861048217e-06</v>
+      </c>
+      <c r="I26" t="n">
+        <v>-1.602763753224874e-06</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-5.462874422439941e-08</v>
       </c>
       <c r="K26" t="n">
-        <v>4.163336342344337e-11</v>
-      </c>
-      <c r="L26" s="4" t="n">
-        <v>-3.59459429772821</v>
-      </c>
-      <c r="M26" s="4" t="n">
-        <v>0.8195204151302538</v>
-      </c>
-      <c r="N26" s="4" t="n">
-        <v>0.3326193625877161</v>
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>-0.0003560517199512622</v>
+      </c>
+      <c r="M26" t="n">
+        <v>-0.0001737364257077932</v>
+      </c>
+      <c r="N26" t="n">
+        <v>-1.308946945967975e-05</v>
       </c>
       <c r="O26" t="n">
-        <v>3.122502256758253e-11</v>
-      </c>
-      <c r="P26" s="2" t="n">
-        <v>0.05199118900331423</v>
-      </c>
-      <c r="Q26" s="2" t="n">
-        <v>-0.5094150819749677</v>
-      </c>
-      <c r="R26" s="2" t="n">
-        <v>-0.4473436647257911</v>
-      </c>
-      <c r="S26" s="2" t="n">
-        <v>-0.01343863506239606</v>
-      </c>
-      <c r="T26" s="2" t="n">
-        <v>-0.009122662122246217</v>
-      </c>
-      <c r="U26" s="2" t="n">
-        <v>0.03229934869911077</v>
-      </c>
-      <c r="V26" s="2" t="n">
-        <v>-0.07763717836672956</v>
-      </c>
-      <c r="W26" s="2" t="n">
-        <v>-0.004190251749747187</v>
-      </c>
-      <c r="X26" s="2" t="n">
-        <v>0.003741888118802272</v>
-      </c>
-      <c r="Y26" s="2" t="n">
-        <v>0.005889499589406544</v>
+        <v>0</v>
+      </c>
+      <c r="P26" s="3" t="n">
+        <v>6.449085363857386e-06</v>
+      </c>
+      <c r="Q26" s="3" t="n">
+        <v>-5.666717669849907e-06</v>
+      </c>
+      <c r="R26" s="3" t="n">
+        <v>4.974126779122712e-06</v>
+      </c>
+      <c r="S26" s="3" t="n">
+        <v>-1.403097688618077e-06</v>
+      </c>
+      <c r="T26" s="3" t="n">
+        <v>-1.01967283729365e-06</v>
+      </c>
+      <c r="U26" s="3" t="n">
+        <v>4.271020732956077e-06</v>
+      </c>
+      <c r="V26" s="3" t="n">
+        <v>4.746056480232172e-06</v>
+      </c>
+      <c r="W26" s="3" t="n">
+        <v>2.462049172499932e-06</v>
+      </c>
+      <c r="X26" s="3" t="n">
+        <v>-6.058169245102765e-10</v>
+      </c>
+      <c r="Y26" s="3" t="n">
+        <v>8.960058980453363e-07</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>0.4722847528580709</v>
-      </c>
-      <c r="AA26" s="2" t="n">
-        <v>-0.01589478064098482</v>
-      </c>
-      <c r="AB26" s="2" t="n">
-        <v>0.01652340148386444</v>
-      </c>
-      <c r="AC26" s="2" t="n">
-        <v>-0.007314916079109723</v>
+        <v>0.9999604516630188</v>
+      </c>
+      <c r="AA26" s="3" t="n">
+        <v>-1.028275720895652e-05</v>
+      </c>
+      <c r="AB26" s="3" t="n">
+        <v>-5.535832419290497e-07</v>
+      </c>
+      <c r="AC26" s="3" t="n">
+        <v>-1.088114993506655e-06</v>
       </c>
     </row>
     <row r="27">
@@ -2880,88 +2880,88 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1.804112415015879e-10</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>44.08768370479932</v>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>-5.638973114119317</v>
-      </c>
-      <c r="F27" s="4" t="n">
-        <v>0.08443888387110743</v>
+        <v>0.00173167152252629</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-0.0004101973407707398</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2.607135319264431e-06</v>
       </c>
       <c r="G27" t="n">
-        <v>1.665334536937735e-10</v>
-      </c>
-      <c r="H27" s="4" t="n">
-        <v>-0.07890478535832468</v>
-      </c>
-      <c r="I27" s="4" t="n">
-        <v>0.4195764605890995</v>
-      </c>
-      <c r="J27" s="4" t="n">
-        <v>-0.1671507187106513</v>
+        <v>-1.363723045079424e-13</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-7.956317830963469e-06</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.0001084910015922079</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-4.851454727858827e-08</v>
       </c>
       <c r="K27" t="n">
-        <v>-1.804112415015879e-10</v>
-      </c>
-      <c r="L27" s="4" t="n">
-        <v>0.3429410156269297</v>
+        <v>0</v>
+      </c>
+      <c r="L27" t="n">
+        <v>-0.0001529780379440198</v>
       </c>
       <c r="M27" s="4" t="n">
-        <v>-5.130312607917742</v>
+        <v>-0.00157248671271009</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>-0.5952864343544695</v>
+        <v>-0.001167294557267457</v>
       </c>
       <c r="O27" t="n">
-        <v>2.775557561562891e-11</v>
-      </c>
-      <c r="P27" s="2" t="n">
-        <v>0.129456103822867</v>
-      </c>
-      <c r="Q27" s="2" t="n">
-        <v>1.0023692691985</v>
-      </c>
-      <c r="R27" s="2" t="n">
-        <v>1.281000773026286</v>
+        <v>0</v>
+      </c>
+      <c r="P27" s="3" t="n">
+        <v>8.359645162484464e-06</v>
+      </c>
+      <c r="Q27" s="3" t="n">
+        <v>7.278208610169985e-05</v>
+      </c>
+      <c r="R27" s="3" t="n">
+        <v>5.274805743001797e-05</v>
       </c>
       <c r="S27" s="3" t="n">
-        <v>-0.0006493931642426176</v>
-      </c>
-      <c r="T27" s="2" t="n">
-        <v>-0.01827062634518484</v>
-      </c>
-      <c r="U27" s="2" t="n">
-        <v>0.009379406848419869</v>
-      </c>
-      <c r="V27" s="2" t="n">
-        <v>0.03806084170054902</v>
-      </c>
-      <c r="W27" s="2" t="n">
-        <v>0.009600667996711998</v>
-      </c>
-      <c r="X27" s="2" t="n">
-        <v>-0.01089037043877639</v>
+        <v>-6.380508054446932e-07</v>
+      </c>
+      <c r="T27" s="3" t="n">
+        <v>-1.235828489629126e-06</v>
+      </c>
+      <c r="U27" s="3" t="n">
+        <v>2.803739315029668e-06</v>
+      </c>
+      <c r="V27" s="3" t="n">
+        <v>2.606121713476451e-06</v>
+      </c>
+      <c r="W27" s="3" t="n">
+        <v>4.765495835114584e-06</v>
+      </c>
+      <c r="X27" s="3" t="n">
+        <v>-1.146852117396222e-09</v>
       </c>
       <c r="Y27" s="3" t="n">
-        <v>0.0002173534546789924</v>
-      </c>
-      <c r="Z27" s="2" t="n">
-        <v>0.1484847070437612</v>
+        <v>5.227492357814413e-07</v>
+      </c>
+      <c r="Z27" s="3" t="n">
+        <v>-1.075893669885732e-05</v>
       </c>
       <c r="AA27" s="2" t="n">
-        <v>0.831404904116928</v>
-      </c>
-      <c r="AB27" s="2" t="n">
-        <v>-0.03852620757138769</v>
-      </c>
-      <c r="AC27" s="2" t="n">
-        <v>-0.003656349001346371</v>
+        <v>0.9999345360855866</v>
+      </c>
+      <c r="AB27" s="3" t="n">
+        <v>-4.928816853421347e-05</v>
+      </c>
+      <c r="AC27" s="3" t="n">
+        <v>-7.71749671953743e-07</v>
       </c>
     </row>
     <row r="28">
@@ -2971,88 +2971,88 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2.359223927328458e-10</v>
+        <v>9.926167350636332e-18</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
-      <c r="D28" s="4" t="n">
-        <v>-44.38938894486822</v>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>5.671406074103658</v>
-      </c>
-      <c r="F28" s="4" t="n">
-        <v>-0.0849831864324635</v>
+      <c r="D28" t="n">
+        <v>-1.341236747611589e-05</v>
+      </c>
+      <c r="E28" t="n">
+        <v>7.766416757277093e-07</v>
+      </c>
+      <c r="F28" t="n">
+        <v>8.563036024245015e-09</v>
       </c>
       <c r="G28" t="n">
-        <v>-4.579669976578771e-10</v>
-      </c>
-      <c r="H28" s="4" t="n">
-        <v>0.08722687505624549</v>
-      </c>
-      <c r="I28" s="4" t="n">
-        <v>-0.4183547842318003</v>
-      </c>
-      <c r="J28" s="4" t="n">
-        <v>0.1675703610592993</v>
+        <v>-1.128704489440857e-13</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-3.125736196456262e-08</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.032020570557183e-07</v>
+      </c>
+      <c r="J28" t="n">
+        <v>-3.378847447647457e-10</v>
       </c>
       <c r="K28" t="n">
-        <v>-2.914335439641036e-10</v>
-      </c>
-      <c r="L28" s="4" t="n">
-        <v>-0.3699885341018616</v>
+        <v>0</v>
+      </c>
+      <c r="L28" t="n">
+        <v>-1.308175190406416e-05</v>
       </c>
       <c r="M28" s="4" t="n">
-        <v>0.2379583333711466</v>
+        <v>-0.001166604455469494</v>
       </c>
       <c r="N28" s="4" t="n">
-        <v>-4.090708081522232</v>
+        <v>-0.001093755018411599</v>
       </c>
       <c r="O28" t="n">
-        <v>-2.220446049250313e-10</v>
-      </c>
-      <c r="P28" s="2" t="n">
-        <v>-0.1299435374857438</v>
-      </c>
-      <c r="Q28" s="2" t="n">
-        <v>-1.006135456282919</v>
-      </c>
-      <c r="R28" s="2" t="n">
-        <v>-1.289758253378293</v>
+        <v>0</v>
+      </c>
+      <c r="P28" s="3" t="n">
+        <v>1.597990861189332e-07</v>
+      </c>
+      <c r="Q28" s="3" t="n">
+        <v>1.685627563029129e-08</v>
+      </c>
+      <c r="R28" s="3" t="n">
+        <v>-4.084262478415719e-07</v>
       </c>
       <c r="S28" s="3" t="n">
-        <v>0.0009799772937579831</v>
-      </c>
-      <c r="T28" s="2" t="n">
-        <v>0.01833211860091666</v>
-      </c>
-      <c r="U28" s="2" t="n">
-        <v>-0.009513510354497434</v>
-      </c>
-      <c r="V28" s="2" t="n">
-        <v>-0.03747636712070346</v>
-      </c>
-      <c r="W28" s="2" t="n">
-        <v>-0.009615814311469961</v>
-      </c>
-      <c r="X28" s="2" t="n">
-        <v>0.01092940470071024</v>
+        <v>2.637413901389237e-08</v>
+      </c>
+      <c r="T28" s="3" t="n">
+        <v>-2.625273180956383e-08</v>
+      </c>
+      <c r="U28" s="3" t="n">
+        <v>5.026433636711507e-08</v>
+      </c>
+      <c r="V28" s="3" t="n">
+        <v>3.590838544075272e-08</v>
+      </c>
+      <c r="W28" s="3" t="n">
+        <v>2.206907322775584e-08</v>
+      </c>
+      <c r="X28" s="3" t="n">
+        <v>-5.383860526756541e-12</v>
       </c>
       <c r="Y28" s="3" t="n">
-        <v>-0.0002506956725545351</v>
-      </c>
-      <c r="Z28" s="2" t="n">
-        <v>-0.1470192326907815</v>
-      </c>
-      <c r="AA28" s="2" t="n">
-        <v>-0.03870667666938665</v>
+        <v>6.810141643450406e-09</v>
+      </c>
+      <c r="Z28" s="3" t="n">
+        <v>-6.166888975616832e-07</v>
+      </c>
+      <c r="AA28" s="3" t="n">
+        <v>-4.930024721316555e-05</v>
       </c>
       <c r="AB28" s="2" t="n">
-        <v>0.8451901878508972</v>
-      </c>
-      <c r="AC28" s="2" t="n">
-        <v>0.003697369646560311</v>
+        <v>0.9999544599201468</v>
+      </c>
+      <c r="AC28" s="3" t="n">
+        <v>-1.157066872842454e-08</v>
       </c>
     </row>
     <row r="29">
@@ -3062,88 +3062,88 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1.994931997373328e-11</v>
+        <v>3.642241673193491e-14</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>-4.167573853324467</v>
+        <v>-0.001180895960499713</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>0.6720439705209733</v>
+        <v>-0.004077420575939131</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>-0.109210589982825</v>
+        <v>-0.00192936203724926</v>
       </c>
       <c r="G29" t="n">
-        <v>2.489328188026718e-10</v>
+        <v>0</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>-0.8019015888876755</v>
+        <v>-0.001031965720020659</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>-0.454664484235423</v>
-      </c>
-      <c r="J29" s="4" t="n">
-        <v>0.01072275455926697</v>
+        <v>0.00115439508237389</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-1.090567978805079e-05</v>
       </c>
       <c r="K29" t="n">
-        <v>9.540979117872439e-12</v>
-      </c>
-      <c r="L29" s="4" t="n">
-        <v>1.030712650072589</v>
+        <v>0</v>
+      </c>
+      <c r="L29" t="n">
+        <v>-0.0008763402812068949</v>
       </c>
       <c r="M29" s="4" t="n">
-        <v>0.9765694065633213</v>
-      </c>
-      <c r="N29" s="4" t="n">
-        <v>0.06035213340454398</v>
+        <v>-0.001928897236878521</v>
+      </c>
+      <c r="N29" t="n">
+        <v>-3.209218256985147e-06</v>
       </c>
       <c r="O29" t="n">
-        <v>8.673617379884035e-13</v>
+        <v>0</v>
       </c>
       <c r="P29" s="2" t="n">
-        <v>0.4387068146321713</v>
-      </c>
-      <c r="Q29" s="2" t="n">
-        <v>-0.130224075791871</v>
-      </c>
-      <c r="R29" s="2" t="n">
-        <v>-0.114557938313449</v>
-      </c>
-      <c r="S29" s="2" t="n">
-        <v>-0.002787843282614499</v>
-      </c>
-      <c r="T29" s="2" t="n">
-        <v>-0.07018529024713921</v>
+        <v>0.005143313278450069</v>
+      </c>
+      <c r="Q29" s="3" t="n">
+        <v>-0.0002622234402211223</v>
+      </c>
+      <c r="R29" s="3" t="n">
+        <v>-3.460940396597159e-05</v>
+      </c>
+      <c r="S29" s="3" t="n">
+        <v>-0.0001674054008958673</v>
+      </c>
+      <c r="T29" s="3" t="n">
+        <v>-0.0008206418817020845</v>
       </c>
       <c r="U29" s="2" t="n">
-        <v>0.06136080871362026</v>
-      </c>
-      <c r="V29" s="2" t="n">
-        <v>-0.05825675407876429</v>
+        <v>0.001160831231223466</v>
+      </c>
+      <c r="V29" s="3" t="n">
+        <v>0.0009297107358080477</v>
       </c>
       <c r="W29" s="3" t="n">
-        <v>-0.0005842564427052666</v>
+        <v>0.0005280490167670525</v>
       </c>
       <c r="X29" s="3" t="n">
-        <v>-0.0003873941523471758</v>
-      </c>
-      <c r="Y29" s="2" t="n">
-        <v>0.005436598790077574</v>
+        <v>-1.295722395158483e-07</v>
+      </c>
+      <c r="Y29" s="3" t="n">
+        <v>0.0001759316796484924</v>
       </c>
       <c r="Z29" s="2" t="n">
-        <v>0.01495094446597039</v>
-      </c>
-      <c r="AA29" s="2" t="n">
-        <v>-0.01585191102427413</v>
-      </c>
-      <c r="AB29" s="2" t="n">
-        <v>0.004809525897334077</v>
+        <v>-0.001741619273231664</v>
+      </c>
+      <c r="AA29" s="3" t="n">
+        <v>-0.0009436907714703545</v>
+      </c>
+      <c r="AB29" s="3" t="n">
+        <v>1.957288114662223e-07</v>
       </c>
       <c r="AC29" s="2" t="n">
-        <v>0.9634955770096432</v>
+        <v>0.9994709354237139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LQR linear ability examination with variety of rotation_y
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -605,88 +605,88 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.9999999999999993</v>
+        <v>1.000000000000001</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>0</v>
+        <v>-2.9778502051909e-17</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>1.799050066851663e-05</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>9.26442286059391e-17</v>
+        <v>1.272120502046882e-05</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>-0.001053211852071116</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>3.026177118578045e-05</v>
+        <v>2.139830361607322e-05</v>
       </c>
       <c r="G2" s="3" t="n">
-        <v>1.919059021123024e-16</v>
+        <v>3.90256615604747e-08</v>
       </c>
       <c r="H2" s="3" t="n">
-        <v>1.496858551907218e-05</v>
+        <v>-8.919465364276281e-06</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>6.105136086874828e-06</v>
+        <v>0.000403624913754845</v>
       </c>
       <c r="J2" s="3" t="n">
-        <v>1.232255564956728e-07</v>
+        <v>1.789407382075424e-08</v>
       </c>
       <c r="K2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L2" s="3" t="n">
-        <v>1.496858551901924e-05</v>
+        <v>3.008824203363208e-05</v>
       </c>
       <c r="M2" s="3" t="n">
-        <v>6.105136086785492e-06</v>
+        <v>-0.0003949909475232203</v>
       </c>
       <c r="N2" s="3" t="n">
-        <v>1.232255558537806e-07</v>
+        <v>1.563731798897815e-07</v>
       </c>
       <c r="O2" s="3" t="n">
-        <v>0</v>
+        <v>-3.308722450212111e-18</v>
       </c>
       <c r="P2" s="4" t="n">
-        <v>0.001998018843353699</v>
+        <v>0.001858784686647587</v>
       </c>
       <c r="Q2" t="n">
-        <v>-1.985233470127266e-16</v>
+        <v>0.0001392341567071806</v>
       </c>
       <c r="R2" t="n">
-        <v>5.418022901891489e-07</v>
+        <v>3.831120727950373e-07</v>
       </c>
       <c r="S2" t="n">
-        <v>5.856438736875436e-16</v>
+        <v>-6.173128452545536e-07</v>
       </c>
       <c r="T2" t="n">
-        <v>3.170844034733207e-07</v>
+        <v>2.242125332871168e-07</v>
       </c>
       <c r="U2" t="n">
-        <v>5.293955920339377e-17</v>
+        <v>-4.074395312005292e-08</v>
       </c>
       <c r="V2" t="n">
-        <v>1.569305089475849e-07</v>
+        <v>-1.662055045296747e-07</v>
       </c>
       <c r="W2" t="n">
-        <v>6.384179521337609e-08</v>
+        <v>1.236990561322861e-05</v>
       </c>
       <c r="X2" t="n">
-        <v>1.356982846576096e-11</v>
+        <v>-2.913544257928741e-09</v>
       </c>
       <c r="Y2" t="n">
-        <v>2.958130122442068e-08</v>
+        <v>8.087841724744384e-08</v>
       </c>
       <c r="Z2" t="n">
-        <v>1.569305087788401e-07</v>
+        <v>3.881387589335939e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>6.384179600416076e-08</v>
+        <v>-1.22796196798644e-05</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.356939833184244e-11</v>
+        <v>2.93273361729522e-09</v>
       </c>
       <c r="AC2" t="n">
-        <v>2.958130116817239e-08</v>
+        <v>-3.904414045772178e-08</v>
       </c>
     </row>
     <row r="3">
@@ -696,88 +696,88 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>3.219509513749243e-18</v>
+        <v>-3.441071348220595e-16</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>3.055885859484022e-16</v>
+        <v>1.272120501898651e-05</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.001489466485253299</v>
+        <v>0.001053211852070408</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>8.421459735278193e-17</v>
+        <v>2.139830361607322e-05</v>
       </c>
       <c r="G3" s="3" t="n">
-        <v>-5.519062642971246e-08</v>
+        <v>-3.902566436958006e-08</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>2.758261440566211e-05</v>
+        <v>3.008824201308492e-05</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>-0.0005647066910612514</v>
+        <v>-0.0003949909475014919</v>
       </c>
       <c r="J3" s="3" t="n">
-        <v>9.791951507300594e-08</v>
+        <v>1.563731795820704e-07</v>
       </c>
       <c r="K3" s="3" t="n">
-        <v>1.52680729448644e-26</v>
+        <v>-6.617444900424221e-18</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>-2.758261440538667e-05</v>
+        <v>-8.919465384648086e-06</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>0.0005647066910606479</v>
+        <v>0.0004036249137783071</v>
       </c>
       <c r="N3" s="3" t="n">
-        <v>-9.791951347700811e-08</v>
+        <v>1.789407326819759e-08</v>
       </c>
       <c r="O3" s="3" t="n">
-        <v>1.526826102396053e-26</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>-6.12476983237632e-16</v>
+        <v>0.0001392341567058869</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>0.001719550529941815</v>
+        <v>0.001858784686645757</v>
       </c>
       <c r="R3" t="n">
-        <v>6.582655066444399e-17</v>
+        <v>3.831120737016273e-07</v>
       </c>
       <c r="S3" t="n">
-        <v>8.73012199837392e-07</v>
+        <v>6.173128454199898e-07</v>
       </c>
       <c r="T3" t="n">
-        <v>7.855749671043616e-16</v>
+        <v>2.242125309114541e-07</v>
       </c>
       <c r="U3" t="n">
-        <v>5.762065200008456e-08</v>
+        <v>4.074395318953609e-08</v>
       </c>
       <c r="V3" t="n">
-        <v>3.91980588624998e-07</v>
+        <v>3.881387590427818e-07</v>
       </c>
       <c r="W3" t="n">
-        <v>-1.742984648754667e-05</v>
+        <v>-1.227961968028461e-05</v>
       </c>
       <c r="X3" t="n">
-        <v>4.13393986383874e-09</v>
+        <v>2.932734772039355e-09</v>
       </c>
       <c r="Y3" t="n">
-        <v>-8.479805312652762e-08</v>
+        <v>-3.904413986546046e-08</v>
       </c>
       <c r="Z3" t="n">
-        <v>-3.919805869990077e-07</v>
+        <v>-1.66205504741433e-07</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.742984648706186e-05</v>
+        <v>1.236990561293083e-05</v>
       </c>
       <c r="AB3" t="n">
-        <v>-4.133940625313281e-09</v>
+        <v>-2.913542927822316e-09</v>
       </c>
       <c r="AC3" t="n">
-        <v>8.479805395969846e-08</v>
+        <v>8.087841830954374e-08</v>
       </c>
     </row>
     <row r="4">
@@ -829,10 +829,10 @@
         <v>0</v>
       </c>
       <c r="P4" t="n">
-        <v>-4.757659544107895e-06</v>
+        <v>-3.364176992537438e-06</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>-3.364176992537438e-06</v>
       </c>
       <c r="R4" s="4" t="n">
         <v>0.001615194096526995</v>
@@ -850,7 +850,7 @@
         <v>-2.011446564864627e-07</v>
       </c>
       <c r="W4" t="n">
-        <v>1.198112442590826e-05</v>
+        <v>1.198113136480217e-05</v>
       </c>
       <c r="X4" t="n">
         <v>-2.844946500601964e-09</v>
@@ -862,7 +862,7 @@
         <v>-2.011446564864627e-07</v>
       </c>
       <c r="AA4" t="n">
-        <v>1.198112442590826e-05</v>
+        <v>1.198113136480217e-05</v>
       </c>
       <c r="AB4" t="n">
         <v>-2.844946500601964e-09</v>
@@ -878,88 +878,88 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>1.673052754524455e-14</v>
+        <v>9.938251146295341e-12</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>2.301517696593952e-16</v>
+        <v>9.938212616460255e-12</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>-1.860739918528885e-14</v>
+        <v>2.81718633866409e-14</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.9892438482012174</v>
+        <v>0.9892438482013315</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>-1.267855515205999e-14</v>
+        <v>1.060895013699557e-14</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>3.944223926405342e-07</v>
+        <v>3.944223025554677e-07</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>-0.0001991766102041677</v>
+        <v>-0.000199176610215269</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>0.004078041405273314</v>
+        <v>0.004078041405055311</v>
       </c>
       <c r="J5" s="3" t="n">
-        <v>-6.920746785633278e-07</v>
+        <v>-6.92074671314169e-07</v>
       </c>
       <c r="K5" s="3" t="n">
-        <v>6.520669004974354e-18</v>
+        <v>9.938211679295212e-12</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>0.0001991766102019097</v>
+        <v>0.0001991766103483976</v>
       </c>
       <c r="M5" s="2" t="n">
-        <v>-0.004078041405225986</v>
+        <v>-0.004078041405342637</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>6.920745941750811e-07</v>
+        <v>6.920746418826206e-07</v>
       </c>
       <c r="O5" s="3" t="n">
-        <v>6.520669004974354e-18</v>
+        <v>9.938211679291351e-12</v>
       </c>
       <c r="P5" t="n">
-        <v>2.259898497556936e-14</v>
+        <v>0.0003771353635518337</v>
       </c>
       <c r="Q5" t="n">
-        <v>-0.0005333499460042509</v>
+        <v>-0.0003771353634659469</v>
       </c>
       <c r="R5" t="n">
-        <v>-1.871774857139237e-15</v>
+        <v>-2.47896289050591e-14</v>
       </c>
       <c r="S5" s="4" t="n">
-        <v>0.001585491060066447</v>
+        <v>0.001585491060123989</v>
       </c>
       <c r="T5" t="n">
-        <v>-3.044364980132614e-14</v>
+        <v>7.572838775901733e-14</v>
       </c>
       <c r="U5" t="n">
-        <v>-9.112615318588796e-07</v>
+        <v>-9.11261406431644e-07</v>
       </c>
       <c r="V5" t="n">
-        <v>-7.921354765130119e-06</v>
+        <v>-7.921354743919724e-06</v>
       </c>
       <c r="W5" t="n">
-        <v>0.0001232485069633201</v>
+        <v>0.0001232485069837873</v>
       </c>
       <c r="X5" t="n">
-        <v>-2.921764308563011e-08</v>
+        <v>-2.921777203600709e-08</v>
       </c>
       <c r="Y5" t="n">
-        <v>-3.485488296203241e-07</v>
+        <v>-3.48548827931494e-07</v>
       </c>
       <c r="Z5" t="n">
-        <v>7.92135468909651e-06</v>
+        <v>7.921354735351466e-06</v>
       </c>
       <c r="AA5" t="n">
-        <v>-0.0001232485069610224</v>
+        <v>-0.0001232485069589014</v>
       </c>
       <c r="AB5" t="n">
-        <v>2.921765670585524e-08</v>
+        <v>2.921771195719315e-08</v>
       </c>
       <c r="AC5" t="n">
-        <v>3.485488156246421e-07</v>
+        <v>3.485488012200516e-07</v>
       </c>
     </row>
     <row r="6">
@@ -975,82 +975,82 @@
         <v>0</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>8.241215373854961e-05</v>
+        <v>8.241215373285236e-05</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>3.71210784615423e-15</v>
+        <v>-1.890865755138903e-14</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>1.00021910609572</v>
+        <v>1.000219106095706</v>
       </c>
       <c r="G6" s="3" t="n">
-        <v>7.265081096321951e-15</v>
+        <v>-1.213042283543141e-14</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>0.000108788260404134</v>
+        <v>0.0001087882603569158</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>4.660869657367959e-05</v>
+        <v>4.660869657041203e-05</v>
       </c>
       <c r="J6" s="3" t="n">
-        <v>1.488720431516092e-06</v>
+        <v>1.488720404954033e-06</v>
       </c>
       <c r="K6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>0.0001087882604022811</v>
+        <v>0.0001087882603671457</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>4.660869656256229e-05</v>
+        <v>4.660869657111118e-05</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>1.488720415369527e-06</v>
+        <v>1.488720426608194e-06</v>
       </c>
       <c r="O6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P6" s="4" t="n">
-        <v>0.002541966837551584</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>-7.23969442799065e-15</v>
+        <v>0.001797441988400008</v>
+      </c>
+      <c r="Q6" s="4" t="n">
+        <v>0.001797441988352147</v>
       </c>
       <c r="R6" t="n">
-        <v>3.861834686948845e-06</v>
+        <v>3.861834679408743e-06</v>
       </c>
       <c r="S6" t="n">
-        <v>2.198477445315336e-14</v>
+        <v>1.002067177367769e-14</v>
       </c>
       <c r="T6" s="4" t="n">
-        <v>0.001594455129139282</v>
+        <v>0.001594455129166929</v>
       </c>
       <c r="U6" t="n">
-        <v>1.888425185228826e-15</v>
+        <v>-1.490591250873484e-14</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.0002005771877196362</v>
+        <v>-0.0002005771876785687</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.0001033384706157853</v>
+        <v>-0.0001033384705887801</v>
       </c>
       <c r="X6" t="n">
-        <v>2.526593204669833e-08</v>
+        <v>2.526594817264593e-08</v>
       </c>
       <c r="Y6" t="n">
-        <v>-3.786088037811842e-05</v>
+        <v>-3.786088038710789e-05</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.0002005771877023249</v>
+        <v>-0.0002005771876980629</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.000103338470594186</v>
+        <v>-0.0001033384705682363</v>
       </c>
       <c r="AB6" t="n">
-        <v>2.526590830330602e-08</v>
+        <v>2.526592469957999e-08</v>
       </c>
       <c r="AC6" t="n">
-        <v>-3.786088037232153e-05</v>
+        <v>-3.786088039128663e-05</v>
       </c>
     </row>
     <row r="7">
@@ -1066,82 +1066,82 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>9.31667374088876e-15</v>
+        <v>9.938211679124081e-12</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>-0.0001348875954676646</v>
+        <v>-0.0001348875476168251</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>-2.124715093493255e-14</v>
+        <v>-4.540921646288955e-11</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>0.9999999999999228</v>
+        <v>0.99999999997267</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>-1.708122517529066e-06</v>
+        <v>-1.708082824846123e-06</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>5.275683340555578e-05</v>
+        <v>5.275676799929345e-05</v>
       </c>
       <c r="J7" s="3" t="n">
-        <v>1.096503081774268e-06</v>
+        <v>1.096518605881396e-06</v>
       </c>
       <c r="K7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>1.708122518862741e-06</v>
+        <v>1.708102701268965e-06</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>-5.275683339151776e-05</v>
+        <v>-5.275674812336211e-05</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>-1.096503096111955e-06</v>
+        <v>-1.096554240609482e-06</v>
       </c>
       <c r="O7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P7" t="n">
-        <v>-3.305523206341751e-15</v>
+        <v>5.649279595285345e-06</v>
       </c>
       <c r="Q7" t="n">
-        <v>-7.989363723988109e-06</v>
+        <v>-5.649246345961064e-06</v>
       </c>
       <c r="R7" t="n">
-        <v>7.661134816082269e-15</v>
+        <v>9.938211679124083e-12</v>
       </c>
       <c r="S7" t="n">
-        <v>-5.18812141603735e-06</v>
+        <v>-5.188170415767112e-06</v>
       </c>
       <c r="T7" t="n">
-        <v>-1.487829301971499e-14</v>
+        <v>-3.677371887886675e-11</v>
       </c>
       <c r="U7" s="4" t="n">
-        <v>0.001614896055877996</v>
+        <v>0.001614896029258542</v>
       </c>
       <c r="V7" t="n">
-        <v>-0.0003739430180996966</v>
+        <v>-0.0003739430453529477</v>
       </c>
       <c r="W7" t="n">
-        <v>-0.0001909196171588882</v>
+        <v>-0.0001909195860762041</v>
       </c>
       <c r="X7" t="n">
-        <v>4.630011212946275e-08</v>
+        <v>4.624645111866485e-08</v>
       </c>
       <c r="Y7" t="n">
-        <v>-7.057116844418313e-05</v>
+        <v>-7.05711931763198e-05</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.00037394301810578</v>
+        <v>0.0003739430096935006</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.0001909196171594517</v>
+        <v>0.0001909196059461839</v>
       </c>
       <c r="AB7" t="n">
-        <v>-4.630009844725853e-08</v>
+        <v>-4.628208584653823e-08</v>
       </c>
       <c r="AC7" t="n">
-        <v>7.057116846065799e-05</v>
+        <v>7.057115754071153e-05</v>
       </c>
     </row>
     <row r="8">
@@ -1151,88 +1151,88 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>2.358757215483243e-19</v>
+        <v>-1.001664023013432e-19</v>
       </c>
       <c r="C8" s="3" t="n">
+        <v>-7.176438048751072e-18</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>3.263908748181676e-07</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>3.136744683952205e-08</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>1.662620441500657e-09</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>1.321259469840072e-16</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0.9999992878965599</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>-3.474728517219194e-07</v>
+      </c>
+      <c r="J8" s="3" t="n">
+        <v>-2.617893890199722e-08</v>
+      </c>
+      <c r="K8" s="3" t="n">
+        <v>3.231174267785264e-21</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>-9.872059722429503e-09</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>-3.205527506920879e-09</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>-1.09257488136564e-10</v>
+      </c>
+      <c r="O8" s="3" t="n">
         <v>-3.231174267785264e-21</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <v>3.263908748192953e-07</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>3.136744661880054e-08</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>1.662620320939083e-09</v>
-      </c>
-      <c r="G8" s="3" t="n">
-        <v>6.086239850800324e-17</v>
-      </c>
-      <c r="H8" s="2" t="n">
-        <v>0.9999992878965601</v>
-      </c>
-      <c r="I8" s="3" t="n">
-        <v>-3.47472851415827e-07</v>
-      </c>
-      <c r="J8" s="3" t="n">
-        <v>-2.617893891926138e-08</v>
-      </c>
-      <c r="K8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="n">
-        <v>-9.872059721734802e-09</v>
-      </c>
-      <c r="M8" s="3" t="n">
-        <v>-3.205527506378042e-09</v>
-      </c>
-      <c r="N8" s="3" t="n">
-        <v>-1.092574880428599e-10</v>
-      </c>
-      <c r="O8" s="3" t="n">
-        <v>0</v>
-      </c>
       <c r="P8" t="n">
-        <v>1.289817072710992e-08</v>
+        <v>1.106435003678111e-09</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.133343533989182e-08</v>
+        <v>1.713433296900594e-08</v>
       </c>
       <c r="R8" t="n">
-        <v>9.94825355865961e-09</v>
+        <v>9.948253558527132e-09</v>
       </c>
       <c r="S8" t="n">
-        <v>2.806195377350718e-09</v>
+        <v>2.806195376872504e-09</v>
       </c>
       <c r="T8" t="n">
-        <v>-2.039345674979021e-09</v>
+        <v>-2.039345674933785e-09</v>
       </c>
       <c r="U8" t="n">
-        <v>-8.542041465607908e-09</v>
+        <v>-8.542041466299379e-09</v>
       </c>
       <c r="V8" s="4" t="n">
-        <v>0.001999920903326038</v>
+        <v>0.001999920903326039</v>
       </c>
       <c r="W8" t="n">
-        <v>-2.056551441794267e-08</v>
+        <v>-2.056551441785866e-08</v>
       </c>
       <c r="X8" t="n">
-        <v>-1.10716648425008e-09</v>
+        <v>-1.107166483833258e-09</v>
       </c>
       <c r="Y8" t="n">
-        <v>-2.176229986960578e-09</v>
+        <v>-2.176229987009045e-09</v>
       </c>
       <c r="Z8" t="n">
-        <v>9.492112961880812e-09</v>
+        <v>9.492112960475252e-09</v>
       </c>
       <c r="AA8" t="n">
-        <v>4.924098344729893e-09</v>
+        <v>4.92409834493992e-09</v>
       </c>
       <c r="AB8" t="n">
-        <v>-1.211633236183117e-12</v>
+        <v>-1.211633291113079e-12</v>
       </c>
       <c r="AC8" t="n">
-        <v>1.792011796281027e-09</v>
+        <v>1.792011796022534e-09</v>
       </c>
     </row>
     <row r="9">
@@ -1245,82 +1245,82 @@
         <v>0</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0</v>
+        <v>-3.226004388956808e-17</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>3.463343045055214e-06</v>
+        <v>3.463343045052733e-06</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>8.203946815456024e-07</v>
+        <v>8.203946817416441e-07</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>5.214270636563481e-09</v>
+        <v>5.214271181675504e-09</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>2.729696021424991e-16</v>
+        <v>-2.555988092788856e-16</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>-3.05956075888847e-07</v>
+        <v>-3.059560755058623e-07</v>
       </c>
       <c r="I9" s="2" t="n">
         <v>0.9999968550265748</v>
       </c>
       <c r="J9" s="3" t="n">
-        <v>-2.334589114533663e-06</v>
+        <v>-2.334589114454254e-06</v>
       </c>
       <c r="K9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>-1.591263566372688e-08</v>
+        <v>-1.591263567778895e-08</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>2.169820031841313e-07</v>
+        <v>2.169820031957118e-07</v>
       </c>
       <c r="N9" s="3" t="n">
-        <v>-9.702909566228984e-11</v>
+        <v>-9.7029093180748e-11</v>
       </c>
       <c r="O9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P9" t="n">
-        <v>1.671929032373808e-08</v>
+        <v>1.147517368288337e-07</v>
       </c>
       <c r="Q9" t="n">
-        <v>-1.455641722021424e-07</v>
+        <v>-9.110708969729012e-08</v>
       </c>
       <c r="R9" t="n">
-        <v>1.054961148597646e-07</v>
+        <v>1.054961148572831e-07</v>
       </c>
       <c r="S9" t="n">
         <v>1.27610161018132e-09</v>
       </c>
       <c r="T9" t="n">
-        <v>-2.471656978881057e-09</v>
+        <v>-2.471656975572335e-09</v>
       </c>
       <c r="U9" t="n">
-        <v>-5.607478631865898e-09</v>
+        <v>-5.607478631038717e-09</v>
       </c>
       <c r="V9" t="n">
         <v>-2.151787339631174e-08</v>
       </c>
       <c r="W9" s="4" t="n">
-        <v>0.001999869072171175</v>
+        <v>0.001999869072171176</v>
       </c>
       <c r="X9" t="n">
-        <v>-9.857633706838063e-08</v>
+        <v>-9.857633707086217e-08</v>
       </c>
       <c r="Y9" t="n">
         <v>-1.543499344397177e-09</v>
       </c>
       <c r="Z9" t="n">
-        <v>5.21224342864035e-09</v>
+        <v>5.212243427813169e-09</v>
       </c>
       <c r="AA9" t="n">
-        <v>9.530991669673302e-09</v>
+        <v>9.530991668018941e-09</v>
       </c>
       <c r="AB9" t="n">
-        <v>-2.293704009799316e-12</v>
+        <v>-2.293703182618704e-12</v>
       </c>
       <c r="AC9" t="n">
         <v>1.045498471860668e-09</v>
@@ -1333,28 +1333,28 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>2.584939414228211e-20</v>
+        <v>1.292469707114106e-20</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0</v>
+        <v>-2.661841361801501e-17</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>-2.682473495223039e-08</v>
+        <v>-2.682473495221746e-08</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>-1.553283351492538e-09</v>
+        <v>-1.553283278455075e-09</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>1.712607203515174e-11</v>
+        <v>1.712652388256135e-11</v>
       </c>
       <c r="G10" s="3" t="n">
-        <v>2.257427590445497e-16</v>
+        <v>-2.324119027332585e-16</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>-2.616350380813675e-08</v>
+        <v>-2.616350333529963e-08</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>-2.333208910938967e-06</v>
+        <v>-2.333208910584669e-06</v>
       </c>
       <c r="J10" s="2" t="n">
         <v>0.9999978124899631</v>
@@ -1363,55 +1363,55 @@
         <v>0</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>-6.251472392529953e-11</v>
+        <v>-6.251472388652544e-11</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>2.064041141083864e-10</v>
+        <v>2.064041141665476e-10</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>-6.757694794999265e-13</v>
+        <v>-6.757694988869721e-13</v>
       </c>
       <c r="O10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P10" t="n">
-        <v>3.195981722381248e-10</v>
+        <v>2.498284084538798e-10</v>
       </c>
       <c r="Q10" t="n">
-        <v>-3.371255126063428e-11</v>
+        <v>2.021516612908502e-10</v>
       </c>
       <c r="R10" t="n">
-        <v>-8.168524956860907e-10</v>
+        <v>-8.168524957571765e-10</v>
       </c>
       <c r="S10" t="n">
         <v>-5.274827806175084e-11</v>
       </c>
       <c r="T10" t="n">
-        <v>-5.250546361964465e-11</v>
+        <v>-5.250546363903169e-11</v>
       </c>
       <c r="U10" t="n">
-        <v>-1.005286727456039e-10</v>
+        <v>-1.005286727068298e-10</v>
       </c>
       <c r="V10" t="n">
-        <v>-1.233377795119541e-09</v>
+        <v>-1.233377795087229e-09</v>
       </c>
       <c r="W10" t="n">
-        <v>-9.860049442631637e-08</v>
+        <v>-9.860049442630991e-08</v>
       </c>
       <c r="X10" s="4" t="n">
         <v>0.001999908919840294</v>
       </c>
       <c r="Y10" t="n">
-        <v>-2.314133745002485e-11</v>
+        <v>-2.314133750172363e-11</v>
       </c>
       <c r="Z10" t="n">
-        <v>7.181677086987321e-11</v>
+        <v>7.181677088926026e-11</v>
       </c>
       <c r="AA10" t="n">
-        <v>4.413814644491343e-11</v>
+        <v>4.413814643845108e-11</v>
       </c>
       <c r="AB10" t="n">
-        <v>-1.076772022633247e-14</v>
+        <v>-1.076771376398393e-14</v>
       </c>
       <c r="AC10" t="n">
         <v>1.362028328426417e-11</v>
@@ -1424,88 +1424,88 @@
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>3.722312756488625e-18</v>
+        <v>8.271806125530277e-19</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0</v>
+        <v>8.271806125530277e-19</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>-2.361791920797229e-06</v>
+        <v>-2.361791920957289e-06</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>8.154841151832739e-06</v>
+        <v>8.154841151723551e-06</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>-3.85872407470422e-06</v>
+        <v>-3.858724074324544e-06</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>-2.067951531382569e-18</v>
+        <v>7.473576834416605e-16</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>-1.752680562429738e-06</v>
+        <v>-1.752680563060877e-06</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>-3.857794473732625e-06</v>
+        <v>-3.857794473453038e-06</v>
       </c>
       <c r="J11" s="3" t="n">
-        <v>-6.418436552602937e-09</v>
+        <v>-6.418437134938088e-09</v>
       </c>
       <c r="K11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>-2.063931440004631e-06</v>
+        <v>-2.063931440711043e-06</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>2.308790164670931e-06</v>
+        <v>2.308790165219766e-06</v>
       </c>
       <c r="N11" s="3" t="n">
-        <v>-2.18113595418166e-08</v>
+        <v>-2.181135991777019e-08</v>
       </c>
       <c r="O11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>1.028662655683098e-05</v>
+        <v>6.902903448497508e-06</v>
       </c>
       <c r="Q11" t="n">
-        <v>5.244468804480547e-07</v>
+        <v>7.644583339509614e-06</v>
       </c>
       <c r="R11" t="n">
-        <v>-6.921880779308271e-08</v>
+        <v>-6.921880783899124e-08</v>
       </c>
       <c r="S11" t="n">
-        <v>3.348108017756841e-07</v>
+        <v>3.348108017785792e-07</v>
       </c>
       <c r="T11" t="n">
-        <v>-1.641283763543079e-06</v>
+        <v>-1.641283763372266e-06</v>
       </c>
       <c r="U11" t="n">
-        <v>-2.321662462411632e-06</v>
+        <v>-2.321662462377304e-06</v>
       </c>
       <c r="V11" t="n">
-        <v>-3.483238546565528e-06</v>
+        <v>-3.48323854630083e-06</v>
       </c>
       <c r="W11" t="n">
-        <v>-1.887381542969975e-06</v>
+        <v>-1.887381542794199e-06</v>
       </c>
       <c r="X11" t="n">
-        <v>3.914576637554622e-10</v>
+        <v>3.914576492798014e-10</v>
       </c>
       <c r="Y11" s="4" t="n">
-        <v>0.001998941870847453</v>
+        <v>0.001998941870847348</v>
       </c>
       <c r="Z11" t="n">
-        <v>1.859421471778613e-06</v>
+        <v>1.859421471563546e-06</v>
       </c>
       <c r="AA11" t="n">
-        <v>1.056098033490996e-06</v>
+        <v>1.056098033524083e-06</v>
       </c>
       <c r="AB11" t="n">
-        <v>-2.591444503186033e-10</v>
+        <v>-2.591443167289343e-10</v>
       </c>
       <c r="AC11" t="n">
-        <v>3.518633594132334e-07</v>
+        <v>3.518633593499541e-07</v>
       </c>
     </row>
     <row r="12">
@@ -1515,88 +1515,88 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>4.297461776154402e-19</v>
+        <v>-7.005185812558453e-18</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>3.231174267785264e-21</v>
+        <v>6.462348535570529e-20</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>3.263908748184164e-07</v>
+        <v>3.263908748182613e-07</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>-3.136744661832878e-08</v>
+        <v>-3.136744640718124e-08</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>1.662620321633785e-09</v>
+        <v>1.662620474015964e-09</v>
       </c>
       <c r="G12" s="3" t="n">
-        <v>-6.196422893331801e-17</v>
+        <v>1.475257235442718e-16</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>-9.872059722096694e-09</v>
+        <v>-9.872059721350292e-09</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>-3.205527506449128e-09</v>
+        <v>-3.205527506849793e-09</v>
       </c>
       <c r="J12" s="3" t="n">
-        <v>-1.092574884499879e-10</v>
+        <v>-1.092574879556182e-10</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L12" s="2" t="n">
-        <v>0.9999992878965601</v>
+        <v>0.9999992878965599</v>
       </c>
       <c r="M12" s="3" t="n">
-        <v>-3.474728514155879e-07</v>
+        <v>-3.474728517489934e-07</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>-2.617893891935831e-08</v>
+        <v>-2.617893908949579e-08</v>
       </c>
       <c r="O12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P12" t="n">
-        <v>1.289817072771415e-08</v>
+        <v>1.713433296926767e-08</v>
       </c>
       <c r="Q12" t="n">
-        <v>-1.133343533970118e-08</v>
+        <v>1.106435003406692e-09</v>
       </c>
       <c r="R12" t="n">
-        <v>9.948253558246019e-09</v>
+        <v>9.948253559031194e-09</v>
       </c>
       <c r="S12" t="n">
-        <v>-2.806195377237627e-09</v>
+        <v>-2.8061953759807e-09</v>
       </c>
       <c r="T12" t="n">
-        <v>-2.039345674588049e-09</v>
+        <v>-2.039345674662366e-09</v>
       </c>
       <c r="U12" t="n">
-        <v>8.542041465911638e-09</v>
+        <v>8.542041465433424e-09</v>
       </c>
       <c r="V12" t="n">
-        <v>9.492112960462328e-09</v>
+        <v>9.492112960074587e-09</v>
       </c>
       <c r="W12" t="n">
-        <v>4.924098344998081e-09</v>
+        <v>4.924098344904377e-09</v>
       </c>
       <c r="X12" t="n">
-        <v>-1.211633850106228e-12</v>
+        <v>-1.211633749939825e-12</v>
       </c>
       <c r="Y12" t="n">
-        <v>1.792011796090388e-09</v>
+        <v>1.792011796329495e-09</v>
       </c>
       <c r="Z12" s="4" t="n">
-        <v>0.001999920903326038</v>
+        <v>0.001999920903326039</v>
       </c>
       <c r="AA12" t="n">
-        <v>-2.056551441791359e-08</v>
+        <v>-2.056551441686669e-08</v>
       </c>
       <c r="AB12" t="n">
-        <v>-1.107166483859108e-09</v>
+        <v>-1.107166484547348e-09</v>
       </c>
       <c r="AC12" t="n">
-        <v>-2.176229987012276e-09</v>
+        <v>-2.176229987719904e-09</v>
       </c>
     </row>
     <row r="13">
@@ -1606,88 +1606,88 @@
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>0</v>
+        <v>-3.226004388956808e-17</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="n">
-        <v>3.463343045051905e-06</v>
+        <v>3.463343045051078e-06</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>-8.203946815414664e-07</v>
+        <v>-8.203946813958826e-07</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>5.214270639045022e-09</v>
+        <v>5.214271327259292e-09</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>-2.729696021424991e-16</v>
+        <v>-1.745351092486888e-16</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>-1.591263566207252e-08</v>
+        <v>-1.59126356628997e-08</v>
       </c>
       <c r="I13" s="3" t="n">
         <v>2.169820031849585e-07</v>
       </c>
       <c r="J13" s="3" t="n">
-        <v>-9.702909483510922e-11</v>
+        <v>-9.702909400792861e-11</v>
       </c>
       <c r="K13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>-3.059560758880198e-07</v>
+        <v>-3.059560754504412e-07</v>
       </c>
       <c r="M13" s="2" t="n">
         <v>0.9999968550265748</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>-2.33458911453449e-06</v>
+        <v>-2.334589114494786e-06</v>
       </c>
       <c r="O13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="P13" t="n">
-        <v>1.671929032456526e-08</v>
+        <v>-9.110708969646294e-08</v>
       </c>
       <c r="Q13" t="n">
-        <v>1.455641722029696e-07</v>
+        <v>1.147517368280065e-07</v>
       </c>
       <c r="R13" t="n">
-        <v>1.054961148597646e-07</v>
+        <v>1.054961148564559e-07</v>
       </c>
       <c r="S13" t="n">
-        <v>-1.2761016110085e-09</v>
+        <v>-1.27610161018132e-09</v>
       </c>
       <c r="T13" t="n">
-        <v>-2.471656978881057e-09</v>
+        <v>-2.471656972263612e-09</v>
       </c>
       <c r="U13" t="n">
-        <v>5.607478630211537e-09</v>
+        <v>5.607478632693078e-09</v>
       </c>
       <c r="V13" t="n">
-        <v>5.212243426985989e-09</v>
+        <v>5.212243427813169e-09</v>
       </c>
       <c r="W13" t="n">
-        <v>9.530991670500483e-09</v>
+        <v>9.530991669673302e-09</v>
       </c>
       <c r="X13" t="n">
         <v>-2.293704009799316e-12</v>
       </c>
       <c r="Y13" t="n">
-        <v>1.045498471860668e-09</v>
+        <v>1.045498471033487e-09</v>
       </c>
       <c r="Z13" t="n">
-        <v>-2.151787339713893e-08</v>
+        <v>-2.151787339631174e-08</v>
       </c>
       <c r="AA13" s="4" t="n">
-        <v>0.001999869072171174</v>
+        <v>0.001999869072171176</v>
       </c>
       <c r="AB13" t="n">
         <v>-9.857633706838063e-08</v>
       </c>
       <c r="AC13" t="n">
-        <v>-1.543499343569996e-09</v>
+        <v>-1.543499345224358e-09</v>
       </c>
     </row>
     <row r="14">
@@ -1697,40 +1697,40 @@
         </is>
       </c>
       <c r="B14" s="3" t="n">
-        <v>2.584939414228211e-20</v>
+        <v>-2.661841361801501e-17</v>
       </c>
       <c r="C14" s="3" t="n">
-        <v>0</v>
+        <v>-1.292469707114106e-20</v>
       </c>
       <c r="D14" s="3" t="n">
-        <v>-2.682473495223039e-08</v>
+        <v>-2.682473495221746e-08</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>1.553283351453764e-09</v>
+        <v>1.553283384515139e-09</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>1.712607204807644e-11</v>
+        <v>1.712664357818092e-11</v>
       </c>
       <c r="G14" s="3" t="n">
-        <v>-2.257427590445497e-16</v>
+        <v>-1.791104520118728e-16</v>
       </c>
       <c r="H14" s="3" t="n">
-        <v>-6.251472392529953e-11</v>
+        <v>-6.251472386713839e-11</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>2.064041141083864e-10</v>
+        <v>2.064041141536229e-10</v>
       </c>
       <c r="J14" s="3" t="n">
-        <v>-6.757694924246236e-13</v>
+        <v>-6.757694794999265e-13</v>
       </c>
       <c r="K14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L14" s="3" t="n">
-        <v>-2.616350380813028e-08</v>
+        <v>-2.616350330871999e-08</v>
       </c>
       <c r="M14" s="3" t="n">
-        <v>-2.333208910938986e-06</v>
+        <v>-2.333208910677643e-06</v>
       </c>
       <c r="N14" s="2" t="n">
         <v>0.9999978124899631</v>
@@ -1739,46 +1739,46 @@
         <v>0</v>
       </c>
       <c r="P14" t="n">
-        <v>3.195981722381248e-10</v>
+        <v>2.021516612585385e-10</v>
       </c>
       <c r="Q14" t="n">
-        <v>3.371255126063428e-11</v>
+        <v>2.498284084409551e-10</v>
       </c>
       <c r="R14" t="n">
-        <v>-8.168524956860907e-10</v>
+        <v>-8.168524957184024e-10</v>
       </c>
       <c r="S14" t="n">
-        <v>5.27482780294391e-11</v>
+        <v>5.274827800358971e-11</v>
       </c>
       <c r="T14" t="n">
-        <v>-5.250546361964465e-11</v>
+        <v>-5.250546365195639e-11</v>
       </c>
       <c r="U14" t="n">
-        <v>1.005286727326792e-10</v>
+        <v>1.005286727132921e-10</v>
       </c>
       <c r="V14" t="n">
-        <v>7.181677087633556e-11</v>
+        <v>7.181677090218496e-11</v>
       </c>
       <c r="W14" t="n">
         <v>4.413814645783813e-11</v>
       </c>
       <c r="X14" t="n">
-        <v>-1.0767726688681e-14</v>
+        <v>-1.076768791458979e-14</v>
       </c>
       <c r="Y14" t="n">
-        <v>1.362028329072652e-11</v>
+        <v>1.362028328426417e-11</v>
       </c>
       <c r="Z14" t="n">
-        <v>-1.233377795126003e-09</v>
+        <v>-1.233377795093691e-09</v>
       </c>
       <c r="AA14" t="n">
-        <v>-9.86004944263293e-08</v>
+        <v>-9.860049442634868e-08</v>
       </c>
       <c r="AB14" s="4" t="n">
         <v>0.001999908919840294</v>
       </c>
       <c r="AC14" t="n">
-        <v>-2.314133745648719e-11</v>
+        <v>-2.314133745002485e-11</v>
       </c>
     </row>
     <row r="15">
@@ -1788,88 +1788,88 @@
         </is>
       </c>
       <c r="B15" s="3" t="n">
-        <v>7.279189390466644e-17</v>
+        <v>-3.391440511467413e-17</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>0</v>
+        <v>8.271806125530277e-19</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>-2.361791920999475e-06</v>
+        <v>-2.361791920945295e-06</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>-8.154841151878234e-06</v>
+        <v>-8.154841152160716e-06</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>-3.858724074498252e-06</v>
+        <v>-3.858724074247616e-06</v>
       </c>
       <c r="G15" s="3" t="n">
-        <v>0</v>
+        <v>3.321130159400406e-16</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>-2.063931440041027e-06</v>
+        <v>-2.063931440919906e-06</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>2.308790164747859e-06</v>
+        <v>2.30879016414319e-06</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>-2.181135957573101e-08</v>
+        <v>-2.181135957821255e-08</v>
       </c>
       <c r="K15" s="3" t="n">
         <v>0</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>-1.752680562413608e-06</v>
+        <v>-1.752680561674936e-06</v>
       </c>
       <c r="M15" s="3" t="n">
-        <v>-3.857794473757027e-06</v>
+        <v>-3.857794474384443e-06</v>
       </c>
       <c r="N15" s="3" t="n">
-        <v>-6.418436514139038e-09</v>
+        <v>-6.418436559220381e-09</v>
       </c>
       <c r="O15" s="2" t="n">
         <v>1</v>
       </c>
       <c r="P15" t="n">
-        <v>1.028662655690046e-05</v>
+        <v>7.64458333939836e-06</v>
       </c>
       <c r="Q15" t="n">
-        <v>-5.244468804422645e-07</v>
+        <v>6.902903448193106e-06</v>
       </c>
       <c r="R15" t="n">
-        <v>-6.921880793204906e-08</v>
+        <v>-6.921880773435289e-08</v>
       </c>
       <c r="S15" t="n">
-        <v>-3.348108017918141e-07</v>
+        <v>-3.348108017397017e-07</v>
       </c>
       <c r="T15" t="n">
-        <v>-1.641283763404113e-06</v>
+        <v>-1.641283763497584e-06</v>
       </c>
       <c r="U15" t="n">
-        <v>2.321662462446787e-06</v>
+        <v>2.321662462266461e-06</v>
       </c>
       <c r="V15" t="n">
-        <v>1.859421471616072e-06</v>
+        <v>1.859421471567269e-06</v>
       </c>
       <c r="W15" t="n">
-        <v>1.056098033534009e-06</v>
+        <v>1.056098033554689e-06</v>
       </c>
       <c r="X15" t="n">
-        <v>-2.591444788563344e-10</v>
+        <v>-2.591443113522604e-10</v>
       </c>
       <c r="Y15" t="n">
-        <v>3.518633592970145e-07</v>
+        <v>3.51863359372288e-07</v>
       </c>
       <c r="Z15" t="n">
-        <v>-3.483238546463371e-06</v>
+        <v>-3.483238546361628e-06</v>
       </c>
       <c r="AA15" t="n">
-        <v>-1.88738154294061e-06</v>
+        <v>-1.887381542699073e-06</v>
       </c>
       <c r="AB15" t="n">
-        <v>3.914576228100218e-10</v>
+        <v>3.914574714359697e-10</v>
       </c>
       <c r="AC15" s="4" t="n">
-        <v>0.001998941870847428</v>
+        <v>0.00199894187084722</v>
       </c>
     </row>
     <row r="16">
@@ -1879,88 +1879,88 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-3.252606517456513e-13</v>
+        <v>2.320870275476783e-13</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>-1.355252715606881e-14</v>
       </c>
       <c r="D16" s="4" t="n">
-        <v>0.008995250334257587</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4.743384504624082e-14</v>
+        <v>0.006360602510233668</v>
+      </c>
+      <c r="E16" s="4" t="n">
+        <v>-0.5266059260355591</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>0.01513088559289022</v>
+        <v>0.01069915180803698</v>
       </c>
       <c r="G16" t="n">
-        <v>9.656175598699024e-14</v>
+        <v>1.951283078055499e-05</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>0.007484292759535837</v>
+        <v>-0.004459732682138246</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>0.003052568043437453</v>
+        <v>0.2018124568774234</v>
       </c>
       <c r="J16" t="n">
-        <v>6.161277824739964e-05</v>
+        <v>8.947036911528556e-06</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
       <c r="L16" s="4" t="n">
-        <v>0.007484292759508732</v>
+        <v>0.01504412101681628</v>
       </c>
       <c r="M16" s="4" t="n">
-        <v>0.003052568043393407</v>
+        <v>-0.1974954737616099</v>
       </c>
       <c r="N16" t="n">
-        <v>6.161277792722118e-05</v>
+        <v>7.81865899453937e-05</v>
       </c>
       <c r="O16" t="n">
-        <v>0</v>
+        <v>-1.694065894508601e-15</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>0.9990094216768499</v>
-      </c>
-      <c r="Q16" s="3" t="n">
-        <v>-9.825582188149884e-14</v>
+        <v>0.9293923433237934</v>
+      </c>
+      <c r="Q16" s="2" t="n">
+        <v>0.06961707835359014</v>
       </c>
       <c r="R16" s="3" t="n">
-        <v>0.0002709011450950774</v>
+        <v>0.0001915560363968834</v>
       </c>
       <c r="S16" s="3" t="n">
-        <v>2.930733997499879e-13</v>
+        <v>-0.0003086564226269592</v>
       </c>
       <c r="T16" s="3" t="n">
-        <v>0.0001585422017363295</v>
+        <v>0.000112106266644154</v>
       </c>
       <c r="U16" s="3" t="n">
-        <v>2.541098841762901e-14</v>
+        <v>-2.037197655984117e-05</v>
       </c>
       <c r="V16" s="3" t="n">
-        <v>7.846525447445421e-05</v>
-      </c>
-      <c r="W16" s="3" t="n">
-        <v>3.192089760648952e-05</v>
+        <v>-8.310275226448003e-05</v>
+      </c>
+      <c r="W16" s="2" t="n">
+        <v>0.006184952806613048</v>
       </c>
       <c r="X16" s="3" t="n">
-        <v>6.784913478491764e-09</v>
+        <v>-1.456772128329096e-06</v>
       </c>
       <c r="Y16" s="3" t="n">
-        <v>1.479065061074127e-05</v>
+        <v>4.043920862405279e-05</v>
       </c>
       <c r="Z16" s="3" t="n">
-        <v>7.846525438975091e-05</v>
-      </c>
-      <c r="AA16" s="3" t="n">
-        <v>3.192089800120688e-05</v>
+        <v>0.000194069379466519</v>
+      </c>
+      <c r="AA16" s="2" t="n">
+        <v>-0.006139809839931975</v>
       </c>
       <c r="AB16" s="3" t="n">
-        <v>6.784700026189056e-09</v>
+        <v>1.466366807641758e-06</v>
       </c>
       <c r="AC16" s="3" t="n">
-        <v>1.479065058363621e-05</v>
+        <v>-1.952207022949616e-05</v>
       </c>
     </row>
     <row r="17">
@@ -1970,88 +1970,88 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1.609754756874604e-15</v>
+        <v>-1.727947212398773e-13</v>
       </c>
       <c r="C17" t="n">
-        <v>-3.016470643570088e-15</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1.527942929742011e-13</v>
+        <v>-5.590417451878382e-14</v>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>0.006360602509493361</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0.7447332426266492</v>
-      </c>
-      <c r="F17" t="n">
-        <v>4.210729867639096e-14</v>
+        <v>0.5266059260352051</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>0.01069915180803529</v>
       </c>
       <c r="G17" t="n">
-        <v>-2.759531321485623e-05</v>
+        <v>-1.951283218493561e-05</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>0.01379130720283105</v>
+        <v>0.01504412100654177</v>
       </c>
       <c r="I17" s="4" t="n">
-        <v>-0.2823533455306256</v>
+        <v>-0.1974954737507459</v>
       </c>
       <c r="J17" t="n">
-        <v>4.895975753650296e-05</v>
+        <v>7.81865897912337e-05</v>
       </c>
       <c r="K17" t="n">
-        <v>7.634049261810735e-24</v>
+        <v>-3.388131789017201e-15</v>
       </c>
       <c r="L17" s="4" t="n">
-        <v>-0.01379130720269334</v>
+        <v>-0.004459732692324665</v>
       </c>
       <c r="M17" s="4" t="n">
-        <v>0.282353345530324</v>
+        <v>0.2018124568891531</v>
       </c>
       <c r="N17" t="n">
-        <v>-4.895975673850405e-05</v>
+        <v>8.947036633701749e-06</v>
       </c>
       <c r="O17" t="n">
-        <v>7.634097410059345e-24</v>
-      </c>
-      <c r="P17" s="3" t="n">
-        <v>-3.06238491618816e-13</v>
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
+        <v>0.0696170783529447</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>0.8597752649709076</v>
+        <v>0.9293923433228786</v>
       </c>
       <c r="R17" s="3" t="n">
-        <v>3.291327533222199e-14</v>
+        <v>0.0001915560368508931</v>
       </c>
       <c r="S17" s="3" t="n">
-        <v>0.000436506099918696</v>
+        <v>0.0003086564227099684</v>
       </c>
       <c r="T17" s="3" t="n">
-        <v>3.927874835521808e-13</v>
+        <v>0.0001121062654566138</v>
       </c>
       <c r="U17" s="3" t="n">
-        <v>2.881032600004228e-05</v>
+        <v>2.037197659541655e-05</v>
       </c>
       <c r="V17" s="3" t="n">
-        <v>0.000195990294312499</v>
+        <v>0.0001940693795224232</v>
       </c>
       <c r="W17" s="2" t="n">
-        <v>-0.008714923243773331</v>
+        <v>-0.006139809840143734</v>
       </c>
       <c r="X17" s="3" t="n">
-        <v>2.066969931919369e-06</v>
+        <v>1.466367387012294e-06</v>
       </c>
       <c r="Y17" s="3" t="n">
-        <v>-4.23990265632638e-05</v>
+        <v>-1.952206993134056e-05</v>
       </c>
       <c r="Z17" s="3" t="n">
-        <v>-0.0001959902934995039</v>
+        <v>-8.310275237120618e-05</v>
       </c>
       <c r="AA17" s="2" t="n">
-        <v>0.008714923243530927</v>
+        <v>0.006184952806465664</v>
       </c>
       <c r="AB17" s="3" t="n">
-        <v>-2.06697031265664e-06</v>
+        <v>-1.456771464255265e-06</v>
       </c>
       <c r="AC17" s="3" t="n">
-        <v>4.239902697984923e-05</v>
+        <v>4.043920915598948e-05</v>
       </c>
     </row>
     <row r="18">
@@ -2061,88 +2061,88 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.641126335305207e-14</v>
+        <v>2.541098841762901e-15</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>3.705769144237564e-15</v>
       </c>
       <c r="D18" s="4" t="n">
-        <v>-6.316815300650524</v>
+        <v>-6.316815300642031</v>
       </c>
       <c r="E18" t="n">
-        <v>-3.398613821739473e-12</v>
+        <v>-2.374582752244546e-11</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>-0.01190378934007634</v>
+        <v>-0.01190378934005898</v>
       </c>
       <c r="G18" t="n">
-        <v>-7.30565917006834e-15</v>
+        <v>1.086503984519668e-10</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>-0.009553995601310029</v>
+        <v>-0.009553995601260688</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>0.1934789676691003</v>
+        <v>0.1934789676640123</v>
       </c>
       <c r="J18" t="n">
-        <v>-3.452787962390781e-05</v>
+        <v>-3.452787959669687e-05</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" s="4" t="n">
-        <v>-0.009553995601308228</v>
+        <v>-0.009553995611456213</v>
       </c>
       <c r="M18" s="4" t="n">
-        <v>0.193478967667414</v>
+        <v>0.1934789676792888</v>
       </c>
       <c r="N18" t="n">
-        <v>-3.452787621227085e-05</v>
+        <v>-3.452787792094807e-05</v>
       </c>
       <c r="O18" t="n">
         <v>0</v>
       </c>
       <c r="P18" s="2" t="n">
-        <v>-0.002378830216249672</v>
-      </c>
-      <c r="Q18" s="3" t="n">
-        <v>7.199780051661553e-15</v>
+        <v>-0.001682086976841219</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>-0.001682086975094425</v>
       </c>
       <c r="R18" s="2" t="n">
-        <v>0.8075970466333712</v>
+        <v>0.807597046626589</v>
       </c>
       <c r="S18" s="3" t="n">
-        <v>-5.115020210231906e-12</v>
+        <v>-5.102632353378312e-12</v>
       </c>
       <c r="T18" s="3" t="n">
-        <v>2.245857666600493e-05</v>
+        <v>2.245857154505549e-05</v>
       </c>
       <c r="U18" s="3" t="n">
-        <v>-1.699465729547347e-12</v>
+        <v>1.712700619348195e-12</v>
       </c>
       <c r="V18" s="3" t="n">
-        <v>-0.0001005734736349581</v>
+        <v>-0.0001005734736767803</v>
       </c>
       <c r="W18" s="2" t="n">
-        <v>0.005990563748253547</v>
+        <v>0.005990563749923366</v>
       </c>
       <c r="X18" s="3" t="n">
-        <v>-1.42238200230031e-06</v>
+        <v>-1.422382018605695e-06</v>
       </c>
       <c r="Y18" s="3" t="n">
-        <v>3.54310710845816e-05</v>
+        <v>3.543106939655082e-05</v>
       </c>
       <c r="Z18" s="3" t="n">
-        <v>-0.0001005734770473362</v>
+        <v>-0.0001005734736568751</v>
       </c>
       <c r="AA18" s="2" t="n">
-        <v>0.00599056374483651</v>
+        <v>0.005990563744810146</v>
       </c>
       <c r="AB18" s="3" t="n">
-        <v>-1.422383675508018e-06</v>
+        <v>-1.422381994677014e-06</v>
       </c>
       <c r="AC18" s="3" t="n">
-        <v>3.543106938098659e-05</v>
+        <v>3.543107109802825e-05</v>
       </c>
     </row>
     <row r="19">
@@ -2152,88 +2152,88 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-2.233950180693945e-13</v>
+        <v>1.395604463389728e-11</v>
       </c>
       <c r="C19" t="n">
-        <v>1.13813954650278e-13</v>
+        <v>1.169347372990463e-12</v>
       </c>
       <c r="D19" t="n">
-        <v>-9.303700511342585e-12</v>
+        <v>1.408140739207472e-11</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>-5.378075886090482</v>
+        <v>-5.378075886033394</v>
       </c>
       <c r="F19" t="n">
-        <v>-6.339295199505375e-12</v>
+        <v>5.322678087002374e-12</v>
       </c>
       <c r="G19" t="n">
-        <v>-9.421011138213063e-12</v>
+        <v>-5.446130656029133e-11</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>-0.0995883049336521</v>
+        <v>-0.09958830493919983</v>
       </c>
       <c r="I19" s="4" t="n">
-        <v>2.039020697434511</v>
+        <v>2.039020697325509</v>
       </c>
       <c r="J19" t="n">
-        <v>-0.0003460374474030068</v>
+        <v>-0.0003460374437873083</v>
       </c>
       <c r="K19" t="n">
-        <v>-2.893825297238485e-22</v>
+        <v>1.392232516987763e-14</v>
       </c>
       <c r="L19" s="4" t="n">
-        <v>0.0995883049325231</v>
+        <v>0.0995883050057703</v>
       </c>
       <c r="M19" s="4" t="n">
-        <v>-2.039020697410847</v>
+        <v>-2.039020697469178</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0003460374052088849</v>
+        <v>0.0003460374290694346</v>
       </c>
       <c r="O19" t="n">
-        <v>-2.893886926996705e-22</v>
-      </c>
-      <c r="P19" s="3" t="n">
-        <v>1.129949280004955e-11</v>
+        <v>-6.442706916728886e-15</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0.1885676812188598</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>-0.266674972214326</v>
+        <v>-0.1885676811759289</v>
       </c>
       <c r="R19" s="3" t="n">
-        <v>-9.358881839883531e-13</v>
+        <v>-1.239692870849386e-11</v>
       </c>
       <c r="S19" s="2" t="n">
-        <v>0.7927455305447909</v>
+        <v>0.7927455305735748</v>
       </c>
       <c r="T19" s="3" t="n">
-        <v>-1.522182343022594e-11</v>
+        <v>3.786119699507839e-11</v>
       </c>
       <c r="U19" s="3" t="n">
-        <v>-0.0004557900037285972</v>
+        <v>-0.0004557899410118524</v>
       </c>
       <c r="V19" s="2" t="n">
-        <v>-0.003960640509688269</v>
+        <v>-0.003960640499081135</v>
       </c>
       <c r="W19" s="2" t="n">
-        <v>0.0616242723074032</v>
+        <v>0.06162427231763335</v>
       </c>
       <c r="X19" s="3" t="n">
-        <v>-1.460882610826533e-05</v>
+        <v>-1.46088905822878e-05</v>
       </c>
       <c r="Y19" s="3" t="n">
-        <v>-0.0001742674560975501</v>
+        <v>-0.0001742674552556333</v>
       </c>
       <c r="Z19" s="2" t="n">
-        <v>0.003960640471671464</v>
+        <v>0.003960640494805236</v>
       </c>
       <c r="AA19" s="2" t="n">
-        <v>-0.06162427230625438</v>
+        <v>-0.06162427230519131</v>
       </c>
       <c r="AB19" s="3" t="n">
-        <v>1.460883291837654e-05</v>
+        <v>1.460886053989779e-05</v>
       </c>
       <c r="AC19" s="3" t="n">
-        <v>0.0001742674490997075</v>
+        <v>0.0001742674418935121</v>
       </c>
     </row>
     <row r="20">
@@ -2243,88 +2243,88 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-8.077306185017008e-12</v>
+        <v>-1.24683249835833e-12</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>-1.802486111757151e-12</v>
       </c>
       <c r="D20" s="4" t="n">
-        <v>0.04120607686926855</v>
+        <v>0.04120607686640897</v>
       </c>
       <c r="E20" t="n">
-        <v>1.870248747537495e-12</v>
+        <v>-9.473216482092095e-12</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0.1095530478601342</v>
+        <v>0.1095530478528023</v>
       </c>
       <c r="G20" t="n">
-        <v>3.618524750670371e-12</v>
+        <v>-6.057979638762756e-12</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0.05439413020204992</v>
+        <v>0.05439413017844141</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>0.02330434828681674</v>
+        <v>0.02330434828516333</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0007443602157585936</v>
+        <v>0.000744360202477117</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>-1.355252715606881e-14</v>
       </c>
       <c r="L20" s="4" t="n">
-        <v>0.05439413020112834</v>
+        <v>0.05439413018357782</v>
       </c>
       <c r="M20" s="4" t="n">
-        <v>0.02330434828128731</v>
+        <v>0.0233043482855699</v>
       </c>
       <c r="N20" t="n">
-        <v>0.0007443602076677349</v>
+        <v>0.0007443602132920337</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>-1.355252715606881e-14</v>
       </c>
       <c r="P20" s="2" t="n">
-        <v>1.270983418775808</v>
-      </c>
-      <c r="Q20" s="3" t="n">
-        <v>-3.63207727782644e-12</v>
+        <v>0.8987209941999753</v>
+      </c>
+      <c r="Q20" s="2" t="n">
+        <v>0.8987209941760822</v>
       </c>
       <c r="R20" s="2" t="n">
-        <v>0.001930917343457629</v>
+        <v>0.001930917339690026</v>
       </c>
       <c r="S20" s="3" t="n">
-        <v>1.09910995235718e-11</v>
+        <v>5.014435047745458e-12</v>
       </c>
       <c r="T20" s="2" t="n">
-        <v>0.7972275645696316</v>
+        <v>0.7972275645834687</v>
       </c>
       <c r="U20" s="3" t="n">
-        <v>9.486769009248164e-13</v>
+        <v>-7.453889935837843e-12</v>
       </c>
       <c r="V20" s="2" t="n">
-        <v>-0.1002885938598445</v>
+        <v>-0.1002885938392717</v>
       </c>
       <c r="W20" s="2" t="n">
-        <v>-0.05166923530788056</v>
+        <v>-0.05166923529439579</v>
       </c>
       <c r="X20" s="3" t="n">
-        <v>1.263296601659511e-05</v>
+        <v>1.263297409390129e-05</v>
       </c>
       <c r="Y20" s="2" t="n">
-        <v>-0.01893044018907324</v>
+        <v>-0.01893044019357269</v>
       </c>
       <c r="Z20" s="2" t="n">
-        <v>-0.1002885938511844</v>
+        <v>-0.1002885938490431</v>
       </c>
       <c r="AA20" s="2" t="n">
-        <v>-0.0516692352970792</v>
+        <v>-0.05166923528415009</v>
       </c>
       <c r="AB20" s="3" t="n">
-        <v>1.263295414458132e-05</v>
+        <v>1.263296234386025e-05</v>
       </c>
       <c r="AC20" s="2" t="n">
-        <v>-0.018930440186173</v>
+        <v>-0.01893044019563267</v>
       </c>
     </row>
     <row r="21">
@@ -2334,88 +2334,88 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>-2.142121267987094e-12</v>
+        <v>4.186699697835617e-12</v>
       </c>
       <c r="C21" t="n">
-        <v>1.667972467202707e-14</v>
+        <v>1.739892248894595e-13</v>
       </c>
       <c r="D21" t="n">
-        <v>4.658335035663008e-12</v>
+        <v>1.457142516141476e-13</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>-0.06724764714273139</v>
+        <v>-0.06724764712419158</v>
       </c>
       <c r="F21" t="n">
-        <v>-1.062352181193065e-11</v>
+        <v>-3.814875693053237e-12</v>
       </c>
       <c r="G21" t="n">
-        <v>4.190231663692277e-13</v>
+        <v>-7.14634187562537e-12</v>
       </c>
       <c r="H21" t="n">
-        <v>-0.0008540808986943678</v>
+        <v>-0.0008540808923638658</v>
       </c>
       <c r="I21" s="4" t="n">
-        <v>0.0263788188205093</v>
+        <v>0.02637881879687951</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0005482514726446857</v>
+        <v>0.0005482514616779788</v>
       </c>
       <c r="K21" t="n">
-        <v>-5.983016928035611e-23</v>
+        <v>7.080181186091445e-17</v>
       </c>
       <c r="L21" t="n">
-        <v>0.000854080899361205</v>
+        <v>0.0008540808873302576</v>
       </c>
       <c r="M21" s="4" t="n">
-        <v>-0.02637881881349029</v>
+        <v>-0.0263788188106568</v>
       </c>
       <c r="N21" t="n">
-        <v>-0.0005482514798135377</v>
+        <v>-0.0005482514731370555</v>
       </c>
       <c r="O21" t="n">
-        <v>-5.983093965233387e-23</v>
-      </c>
-      <c r="P21" s="3" t="n">
-        <v>-1.652759349725905e-12</v>
+        <v>-5.415759298530366e-16</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0.002824703828292213</v>
       </c>
       <c r="Q21" s="2" t="n">
-        <v>-0.00399473445328697</v>
+        <v>-0.002824703804383508</v>
       </c>
       <c r="R21" s="3" t="n">
-        <v>3.830567223485151e-12</v>
+        <v>-5.05331089527233e-12</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>-0.002593904369716818</v>
+        <v>-0.002593904363244654</v>
       </c>
       <c r="T21" s="3" t="n">
-        <v>-7.439149517573695e-12</v>
+        <v>1.089698247837302e-11</v>
       </c>
       <c r="U21" s="2" t="n">
-        <v>0.8074480278491321</v>
+        <v>0.8074480278680549</v>
       </c>
       <c r="V21" s="2" t="n">
-        <v>-0.1869715098309358</v>
+        <v>-0.186971509821892</v>
       </c>
       <c r="W21" s="2" t="n">
-        <v>-0.09545979642644954</v>
+        <v>-0.09545979642122393</v>
       </c>
       <c r="X21" s="3" t="n">
-        <v>2.315005318370776e-05</v>
+        <v>2.31500369878154e-05</v>
       </c>
       <c r="Y21" s="2" t="n">
-        <v>-0.03528558425645998</v>
+        <v>-0.03528558426711281</v>
       </c>
       <c r="Z21" s="2" t="n">
-        <v>0.1869715098339775</v>
+        <v>0.1869715098221494</v>
       </c>
       <c r="AA21" s="2" t="n">
-        <v>0.09545979642673125</v>
+        <v>0.09545979642131602</v>
       </c>
       <c r="AB21" s="3" t="n">
-        <v>-2.315004634260431e-05</v>
+        <v>-2.31500378787727e-05</v>
       </c>
       <c r="AC21" s="2" t="n">
-        <v>0.0352855842646974</v>
+        <v>0.03528558427121013</v>
       </c>
     </row>
     <row r="22">
@@ -2425,88 +2425,88 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.174596469825299e-16</v>
+        <v>-4.963083675318166e-17</v>
       </c>
       <c r="C22" t="n">
+        <v>-3.588309497255034e-15</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0001631954374090834</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1.568372341976123e-05</v>
+      </c>
+      <c r="F22" t="n">
+        <v>8.313102207498246e-07</v>
+      </c>
+      <c r="G22" t="n">
+        <v>6.606360680216011e-14</v>
+      </c>
+      <c r="H22" t="n">
+        <v>-0.000356051720088771</v>
+      </c>
+      <c r="I22" t="n">
+        <v>-0.0001737364258609606</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-1.308946945099766e-05</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1.654361225106055e-18</v>
+      </c>
+      <c r="L22" t="n">
+        <v>-4.936029861213654e-06</v>
+      </c>
+      <c r="M22" t="n">
+        <v>-1.602763753459793e-06</v>
+      </c>
+      <c r="N22" t="n">
+        <v>-5.46287440672351e-08</v>
+      </c>
+      <c r="O22" t="n">
         <v>-1.654361225106055e-18</v>
       </c>
-      <c r="D22" t="n">
-        <v>0.0001631954374096475</v>
-      </c>
-      <c r="E22" t="n">
-        <v>1.568372330940045e-05</v>
-      </c>
-      <c r="F22" t="n">
-        <v>8.313101604698646e-07</v>
-      </c>
-      <c r="G22" t="n">
-        <v>3.043032037460078e-14</v>
-      </c>
-      <c r="H22" t="n">
-        <v>-0.0003560517199515963</v>
-      </c>
-      <c r="I22" t="n">
-        <v>-0.000173736425707914</v>
-      </c>
-      <c r="J22" t="n">
-        <v>-1.308946945963012e-05</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>-4.936029860867891e-06</v>
-      </c>
-      <c r="M22" t="n">
-        <v>-1.602763753188478e-06</v>
-      </c>
-      <c r="N22" t="n">
-        <v>-5.462874402256734e-08</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
       <c r="P22" s="3" t="n">
-        <v>6.449085363554638e-06</v>
+        <v>5.53217501839107e-07</v>
       </c>
       <c r="Q22" s="3" t="n">
-        <v>5.66671766994586e-06</v>
+        <v>8.567166484502363e-06</v>
       </c>
       <c r="R22" s="3" t="n">
-        <v>4.974126779329507e-06</v>
+        <v>4.974126779263333e-06</v>
       </c>
       <c r="S22" s="3" t="n">
-        <v>1.403097688675979e-06</v>
+        <v>1.403097688437751e-06</v>
       </c>
       <c r="T22" s="3" t="n">
-        <v>-1.019672837488864e-06</v>
+        <v>-1.019672837467358e-06</v>
       </c>
       <c r="U22" s="3" t="n">
-        <v>-4.271020732803876e-06</v>
+        <v>-4.271020733149638e-06</v>
       </c>
       <c r="V22" s="2" t="n">
-        <v>0.9999604516630191</v>
+        <v>0.9999604516630193</v>
       </c>
       <c r="W22" s="3" t="n">
-        <v>-1.028275720897141e-05</v>
+        <v>-1.02827572089284e-05</v>
       </c>
       <c r="X22" s="3" t="n">
-        <v>-5.535832421259187e-07</v>
+        <v>-5.535832419174692e-07</v>
       </c>
       <c r="Y22" s="3" t="n">
-        <v>-1.088114993480185e-06</v>
+        <v>-1.088114993505001e-06</v>
       </c>
       <c r="Z22" s="3" t="n">
-        <v>4.746056480940238e-06</v>
+        <v>4.746056480237134e-06</v>
       </c>
       <c r="AA22" s="3" t="n">
-        <v>2.462049172365929e-06</v>
+        <v>2.462049172470154e-06</v>
       </c>
       <c r="AB22" s="3" t="n">
-        <v>-6.058166184534499e-10</v>
+        <v>-6.058166449232295e-10</v>
       </c>
       <c r="AC22" s="3" t="n">
-        <v>8.960058981412892e-07</v>
+        <v>8.960058980105947e-07</v>
       </c>
     </row>
     <row r="23">
@@ -2519,58 +2519,58 @@
         <v>0</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>-1.609362599783171e-14</v>
       </c>
       <c r="D23" s="4" t="n">
-        <v>0.001731671522527984</v>
+        <v>0.00173167152252629</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0004101973407728574</v>
+        <v>0.0004101973408711132</v>
       </c>
       <c r="F23" t="n">
-        <v>2.607135318417398e-06</v>
+        <v>2.60713559073849e-06</v>
       </c>
       <c r="G23" t="n">
-        <v>1.363723045079424e-13</v>
+        <v>-1.274784585617722e-13</v>
       </c>
       <c r="H23" t="n">
-        <v>-0.0001529780379444433</v>
+        <v>-0.0001529780377530139</v>
       </c>
       <c r="I23" s="4" t="n">
-        <v>-0.001572486712709243</v>
+        <v>-0.001572486712589812</v>
       </c>
       <c r="J23" s="4" t="n">
-        <v>-0.001167294557267033</v>
+        <v>-0.001167294557227223</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>-7.956317831810502e-06</v>
+        <v>-7.956317838586765e-06</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0001084910015917844</v>
+        <v>0.0001084910015977136</v>
       </c>
       <c r="N23" t="n">
-        <v>-4.851454770210474e-08</v>
+        <v>-4.85145468550718e-08</v>
       </c>
       <c r="O23" t="n">
         <v>0</v>
       </c>
       <c r="P23" s="3" t="n">
-        <v>8.359645162060947e-06</v>
+        <v>5.737586841446317e-05</v>
       </c>
       <c r="Q23" s="3" t="n">
-        <v>-7.278208610127633e-05</v>
+        <v>-4.555354484882704e-05</v>
       </c>
       <c r="R23" s="3" t="n">
-        <v>5.274805743001797e-05</v>
+        <v>5.27480574283239e-05</v>
       </c>
       <c r="S23" s="3" t="n">
         <v>6.380508050211767e-07</v>
       </c>
       <c r="T23" s="3" t="n">
-        <v>-1.235828489629126e-06</v>
+        <v>-1.23582848793506e-06</v>
       </c>
       <c r="U23" s="3" t="n">
         <v>-2.803739315876701e-06</v>
@@ -2579,22 +2579,22 @@
         <v>-1.07589366984338e-05</v>
       </c>
       <c r="W23" s="2" t="n">
-        <v>0.9999345360855875</v>
+        <v>0.9999345360855879</v>
       </c>
       <c r="X23" s="3" t="n">
-        <v>-4.928816853421347e-05</v>
+        <v>-4.928816853548402e-05</v>
       </c>
       <c r="Y23" s="3" t="n">
-        <v>-7.717496723772595e-07</v>
+        <v>-7.71749671953743e-07</v>
       </c>
       <c r="Z23" s="3" t="n">
-        <v>2.606121714323484e-06</v>
+        <v>2.606121713899967e-06</v>
       </c>
       <c r="AA23" s="3" t="n">
-        <v>4.765495834691067e-06</v>
+        <v>4.765495833844034e-06</v>
       </c>
       <c r="AB23" s="3" t="n">
-        <v>-1.146852117396222e-09</v>
+        <v>-1.146851693879748e-09</v>
       </c>
       <c r="AC23" s="3" t="n">
         <v>5.227492357814413e-07</v>
@@ -2607,85 +2607,85 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1.323488980084844e-17</v>
+        <v>3.308722450212111e-18</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>-1.330768169475311e-14</v>
       </c>
       <c r="D24" t="n">
-        <v>-1.341236747611589e-05</v>
+        <v>-1.341236747610927e-05</v>
       </c>
       <c r="E24" t="n">
-        <v>-7.766416757475616e-07</v>
+        <v>-7.766416392258832e-07</v>
       </c>
       <c r="F24" t="n">
-        <v>8.56303601762757e-09</v>
+        <v>8.563261940505193e-09</v>
       </c>
       <c r="G24" t="n">
-        <v>1.128704489440857e-13</v>
+        <v>-1.162056411738995e-13</v>
       </c>
       <c r="H24" t="n">
-        <v>-1.308175190406747e-05</v>
+        <v>-1.308175166764932e-05</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>-0.001166604455469484</v>
+        <v>-0.001166604455292332</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>-0.001093755018411609</v>
+        <v>-0.001093755018378541</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>-3.12573619612539e-08</v>
+        <v>-3.125736194471028e-08</v>
       </c>
       <c r="M24" t="n">
-        <v>1.032020570557183e-07</v>
+        <v>1.032020570854968e-07</v>
       </c>
       <c r="N24" t="n">
-        <v>-3.378847381473008e-10</v>
+        <v>-3.378847480734682e-10</v>
       </c>
       <c r="O24" t="n">
         <v>0</v>
       </c>
       <c r="P24" s="3" t="n">
-        <v>1.597990861189332e-07</v>
+        <v>1.249142042248203e-07</v>
       </c>
       <c r="Q24" s="3" t="n">
-        <v>-1.685627563029129e-08</v>
+        <v>1.01075830643564e-07</v>
       </c>
       <c r="R24" s="3" t="n">
-        <v>-4.084262478415719e-07</v>
+        <v>-4.084262478779679e-07</v>
       </c>
       <c r="S24" s="3" t="n">
-        <v>-2.637413903043598e-08</v>
+        <v>-2.63741390337447e-08</v>
       </c>
       <c r="T24" s="3" t="n">
-        <v>-2.625273180956383e-08</v>
+        <v>-2.625273181949e-08</v>
       </c>
       <c r="U24" s="3" t="n">
-        <v>-5.026433637373252e-08</v>
+        <v>-5.026433635388018e-08</v>
       </c>
       <c r="V24" s="3" t="n">
-        <v>-6.166888975583745e-07</v>
+        <v>-6.166888975418309e-07</v>
       </c>
       <c r="W24" s="3" t="n">
-        <v>-4.930024721315893e-05</v>
+        <v>-4.930024721315231e-05</v>
       </c>
       <c r="X24" s="2" t="n">
-        <v>0.9999544599201468</v>
+        <v>0.999954459920147</v>
       </c>
       <c r="Y24" s="3" t="n">
-        <v>-1.157066872511582e-08</v>
+        <v>-1.15706687515856e-08</v>
       </c>
       <c r="Z24" s="3" t="n">
-        <v>3.590838543413528e-08</v>
+        <v>3.590838544737017e-08</v>
       </c>
       <c r="AA24" s="3" t="n">
-        <v>2.20690732211384e-08</v>
+        <v>2.206907321782967e-08</v>
       </c>
       <c r="AB24" s="3" t="n">
-        <v>-5.383860526756541e-12</v>
+        <v>-5.38385390931164e-12</v>
       </c>
       <c r="AC24" s="3" t="n">
         <v>6.810141640141684e-09</v>
@@ -2698,88 +2698,88 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.905824131322176e-15</v>
+        <v>4.235164736271502e-16</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>4.235164736271502e-16</v>
       </c>
       <c r="D25" s="4" t="n">
-        <v>-0.001180895960398704</v>
+        <v>-0.001180895960478749</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>0.004077420575916473</v>
+        <v>0.004077420575861628</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>-0.001929362037352174</v>
+        <v>-0.001929362037162227</v>
       </c>
       <c r="G25" t="n">
-        <v>-1.058791184067875e-15</v>
+        <v>3.7375328797596e-13</v>
       </c>
       <c r="H25" t="n">
-        <v>-0.0008763402812149417</v>
+        <v>-0.0008763402815304615</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>-0.001928897236866451</v>
+        <v>-0.001928897236726479</v>
       </c>
       <c r="J25" t="n">
-        <v>-3.209218276466904e-06</v>
+        <v>-3.209218567422722e-06</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>-2.117582368135751e-16</v>
       </c>
       <c r="L25" s="4" t="n">
-        <v>-0.001031965720002448</v>
+        <v>-0.001031965720355449</v>
       </c>
       <c r="M25" s="4" t="n">
-        <v>0.00115439508233535</v>
+        <v>0.001154395082609788</v>
       </c>
       <c r="N25" t="n">
-        <v>-1.090567977089838e-05</v>
+        <v>-1.090567995872793e-05</v>
       </c>
       <c r="O25" t="n">
         <v>0</v>
       </c>
       <c r="P25" s="2" t="n">
-        <v>0.005143313278415341</v>
-      </c>
-      <c r="Q25" s="3" t="n">
-        <v>0.0002622234402240869</v>
+        <v>0.003451451724248762</v>
+      </c>
+      <c r="Q25" s="2" t="n">
+        <v>0.003822291669754817</v>
       </c>
       <c r="R25" s="3" t="n">
-        <v>-3.460940389651489e-05</v>
+        <v>-3.460940391938478e-05</v>
       </c>
       <c r="S25" s="3" t="n">
-        <v>0.0001674054008878205</v>
+        <v>0.0001674054008893028</v>
       </c>
       <c r="T25" s="3" t="n">
-        <v>-0.0008206418817715412</v>
+        <v>-0.0008206418816859908</v>
       </c>
       <c r="U25" s="2" t="n">
-        <v>-0.001160831231205678</v>
+        <v>-0.001160831231188526</v>
       </c>
       <c r="V25" s="2" t="n">
-        <v>-0.001741619273282909</v>
+        <v>-0.00174161927315056</v>
       </c>
       <c r="W25" s="3" t="n">
-        <v>-0.0009436907714851776</v>
+        <v>-0.0009436907713970861</v>
       </c>
       <c r="X25" s="3" t="n">
-        <v>1.957288320067713e-07</v>
+        <v>1.95728824595233e-07</v>
       </c>
       <c r="Y25" s="2" t="n">
-        <v>0.9994709354237266</v>
+        <v>0.9994709354236736</v>
       </c>
       <c r="Z25" s="3" t="n">
-        <v>0.0009297107358893628</v>
+        <v>0.0009297107357817897</v>
       </c>
       <c r="AA25" s="3" t="n">
-        <v>0.0005280490167454532</v>
+        <v>0.0005280490167619703</v>
       </c>
       <c r="AB25" s="3" t="n">
-        <v>-1.295722251162882e-07</v>
+        <v>-1.295721584124436e-07</v>
       </c>
       <c r="AC25" s="3" t="n">
-        <v>0.0001759316797067259</v>
+        <v>0.0001759316796749621</v>
       </c>
     </row>
     <row r="26">
@@ -2789,88 +2789,88 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2.150669592637872e-16</v>
+        <v>-3.502282713549519e-15</v>
       </c>
       <c r="C26" t="n">
-        <v>1.654361225106055e-18</v>
+        <v>3.143286327701505e-17</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0001631954374092074</v>
+        <v>0.0001631954374091297</v>
       </c>
       <c r="E26" t="n">
-        <v>-1.568372330916387e-05</v>
+        <v>-1.568372320359081e-05</v>
       </c>
       <c r="F26" t="n">
-        <v>8.313101608172805e-07</v>
+        <v>8.313102370072323e-07</v>
       </c>
       <c r="G26" t="n">
-        <v>-3.09812226625611e-14</v>
+        <v>7.376300394380369e-14</v>
       </c>
       <c r="H26" t="n">
-        <v>-4.936029861048217e-06</v>
+        <v>-4.936029860675986e-06</v>
       </c>
       <c r="I26" t="n">
-        <v>-1.602763753224874e-06</v>
+        <v>-1.602763753425052e-06</v>
       </c>
       <c r="J26" t="n">
-        <v>-5.462874422439941e-08</v>
+        <v>-5.462874397789959e-08</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>-0.0003560517199512622</v>
+        <v>-0.0003560517200847261</v>
       </c>
       <c r="M26" t="n">
-        <v>-0.0001737364257077932</v>
+        <v>-0.0001737364258744965</v>
       </c>
       <c r="N26" t="n">
-        <v>-1.308946945967975e-05</v>
+        <v>-1.308946954474866e-05</v>
       </c>
       <c r="O26" t="n">
         <v>0</v>
       </c>
       <c r="P26" s="3" t="n">
-        <v>6.449085363857386e-06</v>
+        <v>8.567166484633057e-06</v>
       </c>
       <c r="Q26" s="3" t="n">
-        <v>-5.666717669849907e-06</v>
+        <v>5.532175017034493e-07</v>
       </c>
       <c r="R26" s="3" t="n">
-        <v>4.974126779122712e-06</v>
+        <v>4.97412677951645e-06</v>
       </c>
       <c r="S26" s="3" t="n">
-        <v>-1.403097688618077e-06</v>
+        <v>-1.403097687991074e-06</v>
       </c>
       <c r="T26" s="3" t="n">
-        <v>-1.01967283729365e-06</v>
+        <v>-1.0196728373317e-06</v>
       </c>
       <c r="U26" s="3" t="n">
-        <v>4.271020732956077e-06</v>
+        <v>4.271020732716195e-06</v>
       </c>
       <c r="V26" s="3" t="n">
-        <v>4.746056480232172e-06</v>
+        <v>4.746056480036957e-06</v>
       </c>
       <c r="W26" s="3" t="n">
-        <v>2.462049172499932e-06</v>
+        <v>2.462049172451956e-06</v>
       </c>
       <c r="X26" s="3" t="n">
-        <v>-6.058169245102765e-10</v>
+        <v>-6.058168748794398e-10</v>
       </c>
       <c r="Y26" s="3" t="n">
-        <v>8.960058980453363e-07</v>
+        <v>8.960058981644503e-07</v>
       </c>
       <c r="Z26" s="2" t="n">
-        <v>0.9999604516630188</v>
+        <v>0.9999604516630193</v>
       </c>
       <c r="AA26" s="3" t="n">
-        <v>-1.028275720895652e-05</v>
+        <v>-1.028275720843374e-05</v>
       </c>
       <c r="AB26" s="3" t="n">
-        <v>-5.535832419290497e-07</v>
+        <v>-5.535832422748112e-07</v>
       </c>
       <c r="AC26" s="3" t="n">
-        <v>-1.088114993506655e-06</v>
+        <v>-1.088114993860688e-06</v>
       </c>
     </row>
     <row r="27">
@@ -2880,88 +2880,88 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0</v>
+        <v>-1.609362599783171e-14</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" s="4" t="n">
-        <v>0.00173167152252629</v>
+        <v>0.001731671522525866</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.0004101973407707398</v>
+        <v>-0.000410197340697895</v>
       </c>
       <c r="F27" t="n">
-        <v>2.607135319264431e-06</v>
+        <v>2.607135663583324e-06</v>
       </c>
       <c r="G27" t="n">
-        <v>-1.363723045079424e-13</v>
+        <v>-8.724439356719293e-14</v>
       </c>
       <c r="H27" t="n">
-        <v>-7.956317830963469e-06</v>
+        <v>-7.956317831810502e-06</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0001084910015922079</v>
+        <v>0.0001084910015926314</v>
       </c>
       <c r="J27" t="n">
-        <v>-4.851454727858827e-08</v>
+        <v>-4.85145468550718e-08</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>-0.0001529780379440198</v>
+        <v>-0.0001529780377250618</v>
       </c>
       <c r="M27" s="4" t="n">
-        <v>-0.00157248671271009</v>
+        <v>-0.001572486712658422</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>-0.001167294557267457</v>
+        <v>-0.001167294557247128</v>
       </c>
       <c r="O27" t="n">
         <v>0</v>
       </c>
       <c r="P27" s="3" t="n">
-        <v>8.359645162484464e-06</v>
+        <v>-4.555354484798001e-05</v>
       </c>
       <c r="Q27" s="3" t="n">
-        <v>7.278208610169985e-05</v>
+        <v>5.737586841403965e-05</v>
       </c>
       <c r="R27" s="3" t="n">
-        <v>5.274805743001797e-05</v>
+        <v>5.27480574283239e-05</v>
       </c>
       <c r="S27" s="3" t="n">
-        <v>-6.380508054446932e-07</v>
+        <v>-6.380508050211767e-07</v>
       </c>
       <c r="T27" s="3" t="n">
-        <v>-1.235828489629126e-06</v>
+        <v>-1.235828486240994e-06</v>
       </c>
       <c r="U27" s="3" t="n">
-        <v>2.803739315029668e-06</v>
+        <v>2.803739316300217e-06</v>
       </c>
       <c r="V27" s="3" t="n">
-        <v>2.606121713476451e-06</v>
+        <v>2.606121713899967e-06</v>
       </c>
       <c r="W27" s="3" t="n">
-        <v>4.765495835114584e-06</v>
+        <v>4.765495834691067e-06</v>
       </c>
       <c r="X27" s="3" t="n">
         <v>-1.146852117396222e-09</v>
       </c>
       <c r="Y27" s="3" t="n">
-        <v>5.227492357814413e-07</v>
+        <v>5.227492353579249e-07</v>
       </c>
       <c r="Z27" s="3" t="n">
-        <v>-1.075893669885732e-05</v>
+        <v>-1.07589366984338e-05</v>
       </c>
       <c r="AA27" s="2" t="n">
-        <v>0.9999345360855866</v>
+        <v>0.9999345360855879</v>
       </c>
       <c r="AB27" s="3" t="n">
         <v>-4.928816853421347e-05</v>
       </c>
       <c r="AC27" s="3" t="n">
-        <v>-7.71749671953743e-07</v>
+        <v>-7.71749672800776e-07</v>
       </c>
     </row>
     <row r="28">
@@ -2971,88 +2971,88 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>9.926167350636332e-18</v>
+        <v>-1.330768169475311e-14</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>-3.308722450212111e-18</v>
       </c>
       <c r="D28" t="n">
-        <v>-1.341236747611589e-05</v>
+        <v>-1.341236747610927e-05</v>
       </c>
       <c r="E28" t="n">
-        <v>7.766416757277093e-07</v>
+        <v>7.766416922580866e-07</v>
       </c>
       <c r="F28" t="n">
-        <v>8.563036024245015e-09</v>
+        <v>8.563321788676872e-09</v>
       </c>
       <c r="G28" t="n">
-        <v>-1.128704489440857e-13</v>
+        <v>-8.95571905598912e-14</v>
       </c>
       <c r="H28" t="n">
-        <v>-3.125736196456262e-08</v>
+        <v>-3.125736193478412e-08</v>
       </c>
       <c r="I28" t="n">
-        <v>1.032020570557183e-07</v>
+        <v>1.032020570788794e-07</v>
       </c>
       <c r="J28" t="n">
-        <v>-3.378847447647457e-10</v>
+        <v>-3.378847381473008e-10</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>-1.308175190406416e-05</v>
+        <v>-1.308175165435818e-05</v>
       </c>
       <c r="M28" s="4" t="n">
-        <v>-0.001166604455469494</v>
+        <v>-0.001166604455338823</v>
       </c>
       <c r="N28" s="4" t="n">
-        <v>-0.001093755018411599</v>
+        <v>-0.001093755018355235</v>
       </c>
       <c r="O28" t="n">
         <v>0</v>
       </c>
       <c r="P28" s="3" t="n">
-        <v>1.597990861189332e-07</v>
+        <v>1.010758306270203e-07</v>
       </c>
       <c r="Q28" s="3" t="n">
-        <v>1.685627563029129e-08</v>
+        <v>1.249142042182028e-07</v>
       </c>
       <c r="R28" s="3" t="n">
-        <v>-4.084262478415719e-07</v>
+        <v>-4.084262478581155e-07</v>
       </c>
       <c r="S28" s="3" t="n">
-        <v>2.637413901389237e-08</v>
+        <v>2.63741390039662e-08</v>
       </c>
       <c r="T28" s="3" t="n">
-        <v>-2.625273180956383e-08</v>
+        <v>-2.625273182610744e-08</v>
       </c>
       <c r="U28" s="3" t="n">
-        <v>5.026433636711507e-08</v>
+        <v>5.02643363571889e-08</v>
       </c>
       <c r="V28" s="3" t="n">
-        <v>3.590838544075272e-08</v>
+        <v>3.590838545067889e-08</v>
       </c>
       <c r="W28" s="3" t="n">
         <v>2.206907322775584e-08</v>
       </c>
       <c r="X28" s="3" t="n">
-        <v>-5.383860526756541e-12</v>
+        <v>-5.38384398314429e-12</v>
       </c>
       <c r="Y28" s="3" t="n">
-        <v>6.810141643450406e-09</v>
+        <v>6.810141640141684e-09</v>
       </c>
       <c r="Z28" s="3" t="n">
-        <v>-6.166888975616832e-07</v>
+        <v>-6.166888975484483e-07</v>
       </c>
       <c r="AA28" s="3" t="n">
-        <v>-4.930024721316555e-05</v>
+        <v>-4.930024721317217e-05</v>
       </c>
       <c r="AB28" s="2" t="n">
         <v>0.9999544599201468</v>
       </c>
       <c r="AC28" s="3" t="n">
-        <v>-1.157066872842454e-08</v>
+        <v>-1.157066872511582e-08</v>
       </c>
     </row>
     <row r="29">
@@ -3062,88 +3062,88 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3.642241673193491e-14</v>
+        <v>-1.694065894508601e-14</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>4.235164736271502e-16</v>
       </c>
       <c r="D29" s="4" t="n">
-        <v>-0.001180895960499713</v>
+        <v>-0.001180895960472819</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>-0.004077420575939131</v>
+        <v>-0.004077420576080374</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>-0.00192936203724926</v>
+        <v>-0.001929362037123899</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>1.662302158986564e-13</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>-0.001031965720020659</v>
+        <v>-0.001031965720459846</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>0.00115439508237389</v>
+        <v>0.001154395082071499</v>
       </c>
       <c r="J29" t="n">
-        <v>-1.090567978805079e-05</v>
+        <v>-1.090567978910958e-05</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>-0.0008763402812068949</v>
+        <v>-0.0008763402808373768</v>
       </c>
       <c r="M29" s="4" t="n">
-        <v>-0.001928897236878521</v>
+        <v>-0.001928897237192135</v>
       </c>
       <c r="N29" t="n">
-        <v>-3.209218256985147e-06</v>
+        <v>-3.209218279643278e-06</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
+        <v>-2.117582368135751e-16</v>
       </c>
       <c r="P29" s="2" t="n">
-        <v>0.005143313278450069</v>
-      </c>
-      <c r="Q29" s="3" t="n">
-        <v>-0.0002622234402211223</v>
+        <v>0.003822291669699125</v>
+      </c>
+      <c r="Q29" s="2" t="n">
+        <v>0.00345145172409672</v>
       </c>
       <c r="R29" s="3" t="n">
-        <v>-3.460940396597159e-05</v>
+        <v>-3.460940386729225e-05</v>
       </c>
       <c r="S29" s="3" t="n">
-        <v>-0.0001674054008958673</v>
+        <v>-0.0001674054008698211</v>
       </c>
       <c r="T29" s="3" t="n">
-        <v>-0.0008206418817020845</v>
+        <v>-0.0008206418817486712</v>
       </c>
       <c r="U29" s="2" t="n">
-        <v>0.001160831231223466</v>
+        <v>0.001160831231133257</v>
       </c>
       <c r="V29" s="3" t="n">
-        <v>0.0009297107358080477</v>
+        <v>0.0009297107357836955</v>
       </c>
       <c r="W29" s="3" t="n">
-        <v>0.0005280490167670525</v>
+        <v>0.0005280490167774287</v>
       </c>
       <c r="X29" s="3" t="n">
-        <v>-1.295722395158483e-07</v>
+        <v>-1.295721556595866e-07</v>
       </c>
       <c r="Y29" s="3" t="n">
-        <v>0.0001759316796484924</v>
+        <v>0.0001759316796861853</v>
       </c>
       <c r="Z29" s="2" t="n">
-        <v>-0.001741619273231664</v>
+        <v>-0.00174161927318063</v>
       </c>
       <c r="AA29" s="3" t="n">
-        <v>-0.0009436907714703545</v>
+        <v>-0.0009436907713494406</v>
       </c>
       <c r="AB29" s="3" t="n">
-        <v>1.957288114662223e-07</v>
+        <v>1.957287356567735e-07</v>
       </c>
       <c r="AC29" s="2" t="n">
-        <v>0.9994709354237139</v>
+        <v>0.9994709354236094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>